<commit_message>
Implementada carga de datos
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateu\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreea/Desktop/20-21/1er Cuatrimestre/IC/Sebastián/Genetic_Timetable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE10844-F410-40F3-82AB-9E6F3EBDA4EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF3267D5-409D-6E44-BC07-A668DE647463}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{BC545386-80F0-1D4E-9D05-34C34264D497}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="4" xr2:uid="{BC545386-80F0-1D4E-9D05-34C34264D497}"/>
   </bookViews>
   <sheets>
-    <sheet name="courses_class" sheetId="1" r:id="rId1"/>
-    <sheet name="courses_hours" sheetId="3" r:id="rId2"/>
-    <sheet name="courses_teachers" sheetId="2" r:id="rId3"/>
+    <sheet name="course_classes" sheetId="1" r:id="rId1"/>
+    <sheet name="course_hours" sheetId="3" r:id="rId2"/>
+    <sheet name="class_teachers" sheetId="2" r:id="rId3"/>
     <sheet name="teacher_hours" sheetId="4" r:id="rId4"/>
+    <sheet name="info" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="97">
   <si>
     <t>1 ESO</t>
   </si>
@@ -183,9 +184,6 @@
     <t>Eva M.</t>
   </si>
   <si>
-    <t>Ester C.</t>
-  </si>
-  <si>
     <t>Felip M.</t>
   </si>
   <si>
@@ -198,9 +196,6 @@
     <t>Míriam M.</t>
   </si>
   <si>
-    <t>Maria P.</t>
-  </si>
-  <si>
     <t>Xim H.</t>
   </si>
   <si>
@@ -222,12 +217,6 @@
     <t>Pere V.</t>
   </si>
   <si>
-    <t>Ciencias para el mundo contemporáneo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total profesores </t>
-  </si>
-  <si>
     <t>Ángel F.</t>
   </si>
   <si>
@@ -258,9 +247,6 @@
     <t>Asignatura</t>
   </si>
   <si>
-    <t>Total horas/semana</t>
-  </si>
-  <si>
     <t>1ESO</t>
   </si>
   <si>
@@ -279,15 +265,6 @@
     <t>2BATX</t>
   </si>
   <si>
-    <t>Total horas semanales</t>
-  </si>
-  <si>
-    <t>PROFESORES DE CADA ASIGNATURA</t>
-  </si>
-  <si>
-    <t>HORAS SEMANALES POR ASIGNATURA DE CADA CURSO</t>
-  </si>
-  <si>
     <t>ASIGNATURAS DE CADA CURSO</t>
   </si>
   <si>
@@ -306,9 +283,6 @@
     <t>VIERNES</t>
   </si>
   <si>
-    <t>SEMANA</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -331,13 +305,37 @@
   </si>
   <si>
     <t xml:space="preserve">Yolanda M. </t>
+  </si>
+  <si>
+    <t>Días</t>
+  </si>
+  <si>
+    <t>Horas/día</t>
+  </si>
+  <si>
+    <t>Hora inicio</t>
+  </si>
+  <si>
+    <t>Hora fin</t>
+  </si>
+  <si>
+    <t>Profesor</t>
+  </si>
+  <si>
+    <t>Curso</t>
+  </si>
+  <si>
+    <t>Horas semanales curso</t>
+  </si>
+  <si>
+    <t>Total horas/clase semanales</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -383,6 +381,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="14">
@@ -465,7 +468,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -586,79 +589,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -774,12 +709,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -792,18 +721,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -813,77 +736,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -903,7 +802,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1205,28 +1104,28 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.69921875" customWidth="1"/>
-    <col min="2" max="2" width="29.69921875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="29.69921875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="30.69921875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="29.69921875" style="2" customWidth="1"/>
-    <col min="6" max="7" width="29.69921875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="34.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="29.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="29.6640625" style="2" customWidth="1"/>
+    <col min="6" max="7" width="29.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="47" t="s">
-        <v>83</v>
-      </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-    </row>
-    <row r="2" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+    </row>
+    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="B2" s="23" t="s">
         <v>0</v>
@@ -1247,7 +1146,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="10">
         <v>1</v>
       </c>
@@ -1270,7 +1169,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="31.2">
+    <row r="4" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="10">
         <v>2</v>
       </c>
@@ -1293,7 +1192,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="31.2">
+    <row r="5" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="10">
         <v>3</v>
       </c>
@@ -1316,7 +1215,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="31.2">
+    <row r="6" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="10">
         <v>4</v>
       </c>
@@ -1339,7 +1238,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="10">
         <v>5</v>
       </c>
@@ -1362,7 +1261,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="10">
         <v>6</v>
       </c>
@@ -1385,7 +1284,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="10">
         <v>7</v>
       </c>
@@ -1408,7 +1307,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="10">
         <v>8</v>
       </c>
@@ -1431,7 +1330,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="31.2">
+    <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="10">
         <v>9</v>
       </c>
@@ -1454,7 +1353,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="10">
         <v>10</v>
       </c>
@@ -1475,7 +1374,7 @@
       </c>
       <c r="G12" s="9"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="10">
         <v>11</v>
       </c>
@@ -1494,7 +1393,7 @@
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="10">
         <v>12</v>
       </c>
@@ -1507,7 +1406,7 @@
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
         <v>32</v>
       </c>
@@ -1536,7 +1435,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="30"/>
       <c r="B17" s="30"/>
       <c r="C17" s="30"/>
@@ -1544,7 +1443,7 @@
       <c r="E17" s="30"/>
       <c r="F17" s="25"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="26"/>
       <c r="B18" s="29"/>
       <c r="C18" s="29"/>
@@ -1552,7 +1451,7 @@
       <c r="E18" s="28"/>
       <c r="F18" s="25"/>
     </row>
-    <row r="19" spans="1:6" ht="16.05" customHeight="1">
+    <row r="19" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="40"/>
       <c r="B19" s="29"/>
       <c r="C19" s="29"/>
@@ -1560,7 +1459,7 @@
       <c r="E19" s="29"/>
       <c r="F19" s="25"/>
     </row>
-    <row r="20" spans="1:6" ht="16.05" customHeight="1">
+    <row r="20" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="40"/>
       <c r="B20" s="29"/>
       <c r="C20" s="29"/>
@@ -1568,7 +1467,7 @@
       <c r="E20" s="29"/>
       <c r="F20" s="25"/>
     </row>
-    <row r="21" spans="1:6" ht="16.05" customHeight="1">
+    <row r="21" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="40"/>
       <c r="B21" s="29"/>
       <c r="C21" s="29"/>
@@ -1576,7 +1475,7 @@
       <c r="E21" s="29"/>
       <c r="F21" s="25"/>
     </row>
-    <row r="22" spans="1:6" ht="16.05" customHeight="1">
+    <row r="22" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="40"/>
       <c r="B22" s="29"/>
       <c r="C22" s="29"/>
@@ -1584,7 +1483,7 @@
       <c r="E22" s="29"/>
       <c r="F22" s="25"/>
     </row>
-    <row r="23" spans="1:6" ht="16.05" customHeight="1">
+    <row r="23" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="40"/>
       <c r="B23" s="29"/>
       <c r="C23" s="29"/>
@@ -1592,7 +1491,7 @@
       <c r="E23" s="29"/>
       <c r="F23" s="25"/>
     </row>
-    <row r="24" spans="1:6" ht="16.05" customHeight="1">
+    <row r="24" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="40"/>
       <c r="B24" s="29"/>
       <c r="C24" s="29"/>
@@ -1600,7 +1499,7 @@
       <c r="E24" s="29"/>
       <c r="F24" s="25"/>
     </row>
-    <row r="25" spans="1:6" ht="16.05" customHeight="1">
+    <row r="25" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="40"/>
       <c r="B25" s="29"/>
       <c r="C25" s="29"/>
@@ -1608,7 +1507,7 @@
       <c r="E25" s="29"/>
       <c r="F25" s="25"/>
     </row>
-    <row r="26" spans="1:6" ht="16.05" customHeight="1">
+    <row r="26" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="40"/>
       <c r="B26" s="29"/>
       <c r="C26" s="29"/>
@@ -1616,7 +1515,7 @@
       <c r="E26" s="29"/>
       <c r="F26" s="25"/>
     </row>
-    <row r="27" spans="1:6" ht="16.05" customHeight="1">
+    <row r="27" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="40"/>
       <c r="B27" s="29"/>
       <c r="C27" s="29"/>
@@ -1624,7 +1523,7 @@
       <c r="E27" s="29"/>
       <c r="F27" s="25"/>
     </row>
-    <row r="28" spans="1:6" ht="16.05" customHeight="1">
+    <row r="28" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="40"/>
       <c r="B28" s="29"/>
       <c r="C28" s="29"/>
@@ -1632,7 +1531,7 @@
       <c r="E28" s="29"/>
       <c r="F28" s="25"/>
     </row>
-    <row r="29" spans="1:6" ht="16.05" customHeight="1">
+    <row r="29" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="40"/>
       <c r="B29" s="29"/>
       <c r="C29" s="29"/>
@@ -1640,7 +1539,7 @@
       <c r="E29" s="29"/>
       <c r="F29" s="25"/>
     </row>
-    <row r="30" spans="1:6" ht="16.05" customHeight="1">
+    <row r="30" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="39"/>
       <c r="B30" s="29"/>
       <c r="C30" s="29"/>
@@ -1648,7 +1547,7 @@
       <c r="E30" s="29"/>
       <c r="F30" s="25"/>
     </row>
-    <row r="31" spans="1:6" ht="16.05" customHeight="1">
+    <row r="31" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="39"/>
       <c r="B31" s="29"/>
       <c r="C31" s="29"/>
@@ -1656,7 +1555,7 @@
       <c r="E31" s="29"/>
       <c r="F31" s="25"/>
     </row>
-    <row r="32" spans="1:6" ht="16.05" customHeight="1">
+    <row r="32" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="39"/>
       <c r="B32" s="29"/>
       <c r="C32" s="29"/>
@@ -1664,7 +1563,7 @@
       <c r="E32" s="29"/>
       <c r="F32" s="25"/>
     </row>
-    <row r="33" spans="1:6" ht="16.05" customHeight="1">
+    <row r="33" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="39"/>
       <c r="B33" s="29"/>
       <c r="C33" s="29"/>
@@ -1672,7 +1571,7 @@
       <c r="E33" s="29"/>
       <c r="F33" s="25"/>
     </row>
-    <row r="34" spans="1:6" ht="16.05" customHeight="1">
+    <row r="34" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="39"/>
       <c r="B34" s="29"/>
       <c r="C34" s="29"/>
@@ -1680,7 +1579,7 @@
       <c r="E34" s="29"/>
       <c r="F34" s="25"/>
     </row>
-    <row r="35" spans="1:6" ht="16.05" customHeight="1">
+    <row r="35" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="39"/>
       <c r="B35" s="29"/>
       <c r="C35" s="29"/>
@@ -1688,7 +1587,7 @@
       <c r="E35" s="29"/>
       <c r="F35" s="25"/>
     </row>
-    <row r="36" spans="1:6" ht="16.05" customHeight="1">
+    <row r="36" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="39"/>
       <c r="B36" s="29"/>
       <c r="C36" s="29"/>
@@ -1696,7 +1595,7 @@
       <c r="E36" s="29"/>
       <c r="F36" s="25"/>
     </row>
-    <row r="37" spans="1:6" ht="16.05" customHeight="1">
+    <row r="37" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="39"/>
       <c r="B37" s="29"/>
       <c r="C37" s="29"/>
@@ -1704,7 +1603,7 @@
       <c r="E37" s="29"/>
       <c r="F37" s="25"/>
     </row>
-    <row r="38" spans="1:6" ht="16.05" customHeight="1">
+    <row r="38" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="39"/>
       <c r="B38" s="29"/>
       <c r="C38" s="29"/>
@@ -1712,7 +1611,7 @@
       <c r="E38" s="29"/>
       <c r="F38" s="25"/>
     </row>
-    <row r="39" spans="1:6" ht="16.05" customHeight="1">
+    <row r="39" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="39"/>
       <c r="B39" s="29"/>
       <c r="C39" s="29"/>
@@ -1720,7 +1619,7 @@
       <c r="E39" s="29"/>
       <c r="F39" s="25"/>
     </row>
-    <row r="40" spans="1:6" ht="16.05" customHeight="1">
+    <row r="40" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="39"/>
       <c r="B40" s="29"/>
       <c r="C40" s="29"/>
@@ -1728,7 +1627,7 @@
       <c r="E40" s="29"/>
       <c r="F40" s="25"/>
     </row>
-    <row r="41" spans="1:6" ht="16.05" customHeight="1">
+    <row r="41" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="39"/>
       <c r="B41" s="29"/>
       <c r="C41" s="29"/>
@@ -1736,7 +1635,7 @@
       <c r="E41" s="29"/>
       <c r="F41" s="25"/>
     </row>
-    <row r="42" spans="1:6" ht="16.05" customHeight="1">
+    <row r="42" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="39"/>
       <c r="B42" s="29"/>
       <c r="C42" s="29"/>
@@ -1744,7 +1643,7 @@
       <c r="E42" s="29"/>
       <c r="F42" s="25"/>
     </row>
-    <row r="43" spans="1:6" ht="16.05" customHeight="1">
+    <row r="43" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="39"/>
       <c r="B43" s="29"/>
       <c r="C43" s="29"/>
@@ -1752,7 +1651,7 @@
       <c r="E43" s="29"/>
       <c r="F43" s="25"/>
     </row>
-    <row r="44" spans="1:6" ht="16.05" customHeight="1">
+    <row r="44" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="39"/>
       <c r="B44" s="29"/>
       <c r="C44" s="29"/>
@@ -1760,7 +1659,7 @@
       <c r="E44" s="29"/>
       <c r="F44" s="25"/>
     </row>
-    <row r="45" spans="1:6" ht="16.05" customHeight="1">
+    <row r="45" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="39"/>
       <c r="B45" s="29"/>
       <c r="C45" s="29"/>
@@ -1768,7 +1667,7 @@
       <c r="E45" s="29"/>
       <c r="F45" s="25"/>
     </row>
-    <row r="46" spans="1:6" ht="16.05" customHeight="1">
+    <row r="46" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="39"/>
       <c r="B46" s="29"/>
       <c r="C46" s="29"/>
@@ -1776,7 +1675,7 @@
       <c r="E46" s="29"/>
       <c r="F46" s="25"/>
     </row>
-    <row r="47" spans="1:6" ht="16.05" customHeight="1">
+    <row r="47" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="39"/>
       <c r="B47" s="29"/>
       <c r="C47" s="29"/>
@@ -1784,91 +1683,91 @@
       <c r="E47" s="28"/>
       <c r="F47" s="25"/>
     </row>
-    <row r="48" spans="1:6" ht="16.05" customHeight="1">
+    <row r="48" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="39"/>
       <c r="B48" s="38"/>
       <c r="C48" s="38"/>
       <c r="D48" s="38"/>
     </row>
-    <row r="49" spans="1:6" ht="16.95" customHeight="1">
+    <row r="49" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="39"/>
       <c r="B49" s="38"/>
       <c r="C49" s="38"/>
       <c r="D49" s="38"/>
     </row>
-    <row r="50" spans="1:6" ht="16.95" customHeight="1">
+    <row r="50" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="39"/>
       <c r="B50" s="29"/>
       <c r="C50" s="29"/>
       <c r="D50" s="38"/>
     </row>
-    <row r="51" spans="1:6" ht="16.05" customHeight="1">
+    <row r="51" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="39"/>
       <c r="B51" s="29"/>
       <c r="C51" s="29"/>
       <c r="D51" s="38"/>
     </row>
-    <row r="52" spans="1:6" ht="16.05" customHeight="1">
+    <row r="52" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="39"/>
       <c r="B52" s="29"/>
       <c r="C52" s="29"/>
       <c r="D52" s="38"/>
     </row>
-    <row r="53" spans="1:6" ht="16.05" customHeight="1">
+    <row r="53" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="39"/>
       <c r="B53" s="29"/>
       <c r="C53" s="29"/>
       <c r="D53" s="38"/>
     </row>
-    <row r="54" spans="1:6" ht="16.05" customHeight="1">
+    <row r="54" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="39"/>
       <c r="B54" s="29"/>
       <c r="C54" s="29"/>
       <c r="D54" s="38"/>
     </row>
-    <row r="55" spans="1:6" ht="16.05" customHeight="1">
+    <row r="55" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="39"/>
       <c r="B55" s="29"/>
       <c r="C55" s="29"/>
       <c r="D55" s="38"/>
     </row>
-    <row r="56" spans="1:6" ht="16.05" customHeight="1">
+    <row r="56" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="39"/>
       <c r="B56" s="29"/>
       <c r="C56" s="29"/>
       <c r="D56" s="38"/>
     </row>
-    <row r="57" spans="1:6" ht="16.05" customHeight="1">
+    <row r="57" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="39"/>
       <c r="B57" s="29"/>
       <c r="C57" s="29"/>
       <c r="D57" s="38"/>
     </row>
-    <row r="58" spans="1:6" ht="16.05" customHeight="1">
+    <row r="58" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="39"/>
       <c r="B58" s="29"/>
       <c r="C58" s="29"/>
       <c r="D58" s="38"/>
     </row>
-    <row r="59" spans="1:6" ht="16.05" customHeight="1">
+    <row r="59" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="39"/>
       <c r="B59" s="29"/>
       <c r="C59" s="29"/>
       <c r="D59" s="38"/>
     </row>
-    <row r="60" spans="1:6" ht="16.05" customHeight="1">
+    <row r="60" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="39"/>
       <c r="B60" s="29"/>
       <c r="C60" s="29"/>
       <c r="D60" s="38"/>
     </row>
-    <row r="61" spans="1:6" ht="16.05" customHeight="1">
+    <row r="61" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="39"/>
       <c r="B61" s="29"/>
       <c r="C61" s="29"/>
       <c r="D61" s="38"/>
     </row>
-    <row r="62" spans="1:6" ht="16.05" customHeight="1">
+    <row r="62" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="39"/>
       <c r="B62" s="29"/>
       <c r="C62" s="29"/>
@@ -1876,7 +1775,7 @@
       <c r="E62" s="13"/>
       <c r="F62" s="16"/>
     </row>
-    <row r="63" spans="1:6" ht="16.05" customHeight="1">
+    <row r="63" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="39"/>
       <c r="B63" s="29"/>
       <c r="C63" s="29"/>
@@ -1884,7 +1783,7 @@
       <c r="E63" s="13"/>
       <c r="F63" s="16"/>
     </row>
-    <row r="64" spans="1:6" ht="16.05" customHeight="1">
+    <row r="64" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="39"/>
       <c r="B64" s="29"/>
       <c r="C64" s="29"/>
@@ -1892,7 +1791,7 @@
       <c r="E64" s="13"/>
       <c r="F64" s="16"/>
     </row>
-    <row r="65" spans="1:6" ht="16.05" customHeight="1">
+    <row r="65" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="39"/>
       <c r="B65" s="29"/>
       <c r="C65" s="29"/>
@@ -1900,7 +1799,7 @@
       <c r="E65" s="13"/>
       <c r="F65" s="16"/>
     </row>
-    <row r="66" spans="1:6" ht="16.05" customHeight="1">
+    <row r="66" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="39"/>
       <c r="B66" s="29"/>
       <c r="C66" s="29"/>
@@ -1908,7 +1807,7 @@
       <c r="E66" s="13"/>
       <c r="F66" s="16"/>
     </row>
-    <row r="67" spans="1:6" ht="16.05" customHeight="1">
+    <row r="67" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="39"/>
       <c r="B67" s="29"/>
       <c r="C67" s="29"/>
@@ -1916,7 +1815,7 @@
       <c r="E67" s="13"/>
       <c r="F67" s="16"/>
     </row>
-    <row r="68" spans="1:6" ht="16.05" customHeight="1">
+    <row r="68" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="39"/>
       <c r="B68" s="29"/>
       <c r="C68" s="29"/>
@@ -1924,7 +1823,7 @@
       <c r="E68" s="13"/>
       <c r="F68" s="16"/>
     </row>
-    <row r="69" spans="1:6" ht="16.05" customHeight="1">
+    <row r="69" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="39"/>
       <c r="B69" s="29"/>
       <c r="C69" s="29"/>
@@ -1932,7 +1831,7 @@
       <c r="E69" s="13"/>
       <c r="F69" s="16"/>
     </row>
-    <row r="70" spans="1:6" ht="16.05" customHeight="1">
+    <row r="70" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="39"/>
       <c r="B70" s="29"/>
       <c r="C70" s="29"/>
@@ -1940,7 +1839,7 @@
       <c r="E70" s="13"/>
       <c r="F70" s="16"/>
     </row>
-    <row r="71" spans="1:6" ht="16.05" customHeight="1">
+    <row r="71" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="39"/>
       <c r="B71" s="29"/>
       <c r="C71" s="29"/>
@@ -1948,7 +1847,7 @@
       <c r="E71" s="13"/>
       <c r="F71" s="16"/>
     </row>
-    <row r="72" spans="1:6" ht="16.05" customHeight="1">
+    <row r="72" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="39"/>
       <c r="B72" s="29"/>
       <c r="C72" s="29"/>
@@ -1956,7 +1855,7 @@
       <c r="E72" s="13"/>
       <c r="F72" s="16"/>
     </row>
-    <row r="73" spans="1:6" ht="16.05" customHeight="1">
+    <row r="73" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="39"/>
       <c r="B73" s="29"/>
       <c r="C73" s="29"/>
@@ -1964,7 +1863,7 @@
       <c r="E73" s="13"/>
       <c r="F73" s="16"/>
     </row>
-    <row r="74" spans="1:6" ht="16.05" customHeight="1">
+    <row r="74" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="39"/>
       <c r="B74" s="29"/>
       <c r="C74" s="29"/>
@@ -1972,7 +1871,7 @@
       <c r="E74" s="13"/>
       <c r="F74" s="16"/>
     </row>
-    <row r="75" spans="1:6" ht="16.05" customHeight="1">
+    <row r="75" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="39"/>
       <c r="B75" s="29"/>
       <c r="C75" s="29"/>
@@ -1980,7 +1879,7 @@
       <c r="E75" s="13"/>
       <c r="F75" s="16"/>
     </row>
-    <row r="76" spans="1:6" ht="16.05" customHeight="1">
+    <row r="76" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="39"/>
       <c r="B76" s="29"/>
       <c r="C76" s="29"/>
@@ -1988,7 +1887,7 @@
       <c r="E76" s="13"/>
       <c r="F76" s="16"/>
     </row>
-    <row r="77" spans="1:6" ht="16.05" customHeight="1">
+    <row r="77" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="39"/>
       <c r="B77" s="29"/>
       <c r="C77" s="29"/>
@@ -1996,7 +1895,7 @@
       <c r="E77" s="13"/>
       <c r="F77" s="16"/>
     </row>
-    <row r="78" spans="1:6" ht="16.05" customHeight="1">
+    <row r="78" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="39"/>
       <c r="B78" s="29"/>
       <c r="C78" s="29"/>
@@ -2004,7 +1903,7 @@
       <c r="E78" s="13"/>
       <c r="F78" s="16"/>
     </row>
-    <row r="79" spans="1:6" ht="16.05" customHeight="1">
+    <row r="79" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="39"/>
       <c r="B79" s="29"/>
       <c r="C79" s="29"/>
@@ -2012,7 +1911,7 @@
       <c r="E79" s="13"/>
       <c r="F79" s="16"/>
     </row>
-    <row r="80" spans="1:6" ht="16.05" customHeight="1">
+    <row r="80" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="39"/>
       <c r="B80" s="29"/>
       <c r="C80" s="29"/>
@@ -2020,7 +1919,7 @@
       <c r="E80" s="13"/>
       <c r="F80" s="16"/>
     </row>
-    <row r="81" spans="1:6" ht="16.05" customHeight="1">
+    <row r="81" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="39"/>
       <c r="B81" s="29"/>
       <c r="C81" s="29"/>
@@ -2028,7 +1927,7 @@
       <c r="E81" s="13"/>
       <c r="F81" s="16"/>
     </row>
-    <row r="82" spans="1:6" ht="16.05" customHeight="1">
+    <row r="82" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="39"/>
       <c r="B82" s="29"/>
       <c r="C82" s="29"/>
@@ -2036,7 +1935,7 @@
       <c r="E82" s="13"/>
       <c r="F82" s="16"/>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="12"/>
       <c r="B83" s="14"/>
       <c r="C83" s="14"/>
@@ -2044,7 +1943,7 @@
       <c r="E83" s="13"/>
       <c r="F83" s="16"/>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="12"/>
       <c r="B84" s="14"/>
       <c r="C84" s="14"/>
@@ -2052,7 +1951,7 @@
       <c r="E84" s="13"/>
       <c r="F84" s="16"/>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="12"/>
       <c r="B85" s="14"/>
       <c r="C85" s="14"/>
@@ -2060,7 +1959,7 @@
       <c r="E85" s="13"/>
       <c r="F85" s="16"/>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="12"/>
       <c r="B86" s="14"/>
       <c r="C86" s="14"/>
@@ -2068,7 +1967,7 @@
       <c r="E86" s="13"/>
       <c r="F86" s="16"/>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="12"/>
       <c r="B87" s="14"/>
       <c r="C87" s="14"/>
@@ -2076,7 +1975,7 @@
       <c r="E87" s="13"/>
       <c r="F87" s="16"/>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="12"/>
       <c r="B88" s="14"/>
       <c r="C88" s="14"/>
@@ -2084,7 +1983,7 @@
       <c r="E88" s="13"/>
       <c r="F88" s="16"/>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="12"/>
       <c r="B89" s="14"/>
       <c r="C89" s="14"/>
@@ -2092,7 +1991,7 @@
       <c r="E89" s="13"/>
       <c r="F89" s="16"/>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="12"/>
       <c r="B90" s="14"/>
       <c r="C90" s="14"/>
@@ -2100,7 +1999,7 @@
       <c r="E90" s="13"/>
       <c r="F90" s="16"/>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="12"/>
       <c r="B91" s="14"/>
       <c r="C91" s="14"/>
@@ -2108,7 +2007,7 @@
       <c r="E91" s="13"/>
       <c r="F91" s="16"/>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="12"/>
       <c r="B92" s="14"/>
       <c r="C92" s="14"/>
@@ -2116,7 +2015,7 @@
       <c r="E92" s="13"/>
       <c r="F92" s="16"/>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="12"/>
       <c r="B93" s="14"/>
       <c r="C93" s="14"/>
@@ -2124,7 +2023,7 @@
       <c r="E93" s="13"/>
       <c r="F93" s="16"/>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="12"/>
       <c r="B94" s="14"/>
       <c r="C94" s="14"/>
@@ -2132,7 +2031,7 @@
       <c r="E94" s="13"/>
       <c r="F94" s="16"/>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="12"/>
       <c r="B95" s="14"/>
       <c r="C95" s="14"/>
@@ -2140,7 +2039,7 @@
       <c r="E95" s="13"/>
       <c r="F95" s="16"/>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="12"/>
       <c r="B96" s="14"/>
       <c r="C96" s="14"/>
@@ -2148,7 +2047,7 @@
       <c r="E96" s="13"/>
       <c r="F96" s="16"/>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="12"/>
       <c r="B97" s="14"/>
       <c r="C97" s="14"/>
@@ -2156,7 +2055,7 @@
       <c r="E97" s="13"/>
       <c r="F97" s="16"/>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" s="12"/>
       <c r="B98" s="14"/>
       <c r="C98" s="14"/>
@@ -2164,7 +2063,7 @@
       <c r="E98" s="13"/>
       <c r="F98" s="16"/>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="12"/>
       <c r="B99" s="14"/>
       <c r="C99" s="14"/>
@@ -2172,7 +2071,7 @@
       <c r="E99" s="13"/>
       <c r="F99" s="16"/>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="12"/>
       <c r="B100" s="14"/>
       <c r="C100" s="14"/>
@@ -2180,147 +2079,147 @@
       <c r="E100" s="13"/>
       <c r="F100" s="16"/>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" s="12"/>
       <c r="B101" s="14"/>
       <c r="C101" s="14"/>
       <c r="E101" s="13"/>
       <c r="F101" s="16"/>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" s="12"/>
       <c r="B102" s="13"/>
       <c r="C102" s="14"/>
       <c r="E102" s="13"/>
       <c r="F102" s="16"/>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" s="12"/>
       <c r="B103" s="13"/>
       <c r="C103" s="14"/>
       <c r="E103" s="13"/>
       <c r="F103" s="16"/>
     </row>
-    <row r="104" spans="1:6">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" s="12"/>
       <c r="B104" s="13"/>
       <c r="C104" s="14"/>
       <c r="E104" s="13"/>
       <c r="F104" s="16"/>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" s="12"/>
       <c r="B105" s="13"/>
       <c r="C105" s="14"/>
       <c r="E105" s="13"/>
       <c r="F105" s="16"/>
     </row>
-    <row r="106" spans="1:6">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C106" s="14"/>
       <c r="E106" s="13"/>
       <c r="F106" s="16"/>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E107" s="13"/>
       <c r="F107" s="16"/>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E108" s="13"/>
       <c r="F108" s="16"/>
     </row>
-    <row r="109" spans="1:6">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E109" s="13"/>
       <c r="F109" s="16"/>
     </row>
-    <row r="110" spans="1:6">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E110" s="13"/>
       <c r="F110" s="16"/>
     </row>
-    <row r="111" spans="1:6">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E111" s="13"/>
       <c r="F111" s="16"/>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E112" s="13"/>
       <c r="F112" s="16"/>
     </row>
-    <row r="113" spans="5:6">
+    <row r="113" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E113" s="13"/>
       <c r="F113" s="16"/>
     </row>
-    <row r="114" spans="5:6">
+    <row r="114" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E114" s="13"/>
       <c r="F114" s="16"/>
     </row>
-    <row r="115" spans="5:6">
+    <row r="115" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E115" s="13"/>
       <c r="F115" s="16"/>
     </row>
-    <row r="116" spans="5:6">
+    <row r="116" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E116" s="13"/>
       <c r="F116" s="16"/>
     </row>
-    <row r="117" spans="5:6">
+    <row r="117" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E117" s="13"/>
       <c r="F117" s="16"/>
     </row>
-    <row r="118" spans="5:6">
+    <row r="118" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E118" s="13"/>
       <c r="F118" s="16"/>
     </row>
-    <row r="119" spans="5:6">
+    <row r="119" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E119" s="13"/>
       <c r="F119" s="16"/>
     </row>
-    <row r="120" spans="5:6">
+    <row r="120" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E120" s="13"/>
       <c r="F120" s="16"/>
     </row>
-    <row r="121" spans="5:6">
+    <row r="121" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E121" s="13"/>
       <c r="F121" s="16"/>
     </row>
-    <row r="122" spans="5:6">
+    <row r="122" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E122" s="13"/>
       <c r="F122" s="16"/>
     </row>
-    <row r="123" spans="5:6">
+    <row r="123" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E123" s="13"/>
       <c r="F123" s="16"/>
     </row>
-    <row r="124" spans="5:6">
+    <row r="124" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E124" s="13"/>
       <c r="F124" s="16"/>
     </row>
-    <row r="125" spans="5:6">
+    <row r="125" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E125" s="13"/>
       <c r="F125" s="16"/>
     </row>
-    <row r="126" spans="5:6">
+    <row r="126" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E126" s="13"/>
       <c r="F126" s="16"/>
     </row>
-    <row r="127" spans="5:6">
+    <row r="127" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E127" s="13"/>
       <c r="F127" s="16"/>
     </row>
-    <row r="128" spans="5:6">
+    <row r="128" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E128" s="13"/>
       <c r="F128" s="16"/>
     </row>
-    <row r="129" spans="5:6">
+    <row r="129" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E129" s="13"/>
       <c r="F129" s="16"/>
     </row>
-    <row r="130" spans="5:6">
+    <row r="130" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E130" s="13"/>
       <c r="F130" s="16"/>
     </row>
-    <row r="131" spans="5:6">
+    <row r="131" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E131" s="13"/>
       <c r="F131" s="16"/>
     </row>
-    <row r="132" spans="5:6">
+    <row r="132" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E132" s="13"/>
       <c r="F132" s="16"/>
     </row>
@@ -2340,719 +2239,824 @@
   <dimension ref="A1:D66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="35.296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="35.33203125" style="55" customWidth="1"/>
+    <col min="2" max="4" width="35.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="60" t="s">
-        <v>82</v>
-      </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="62"/>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="16"/>
-      <c r="B2" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="63" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" s="17" t="s">
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="54" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>33</v>
+      </c>
+      <c r="C2" s="9">
+        <v>3</v>
+      </c>
+      <c r="D2" s="48">
+        <f>SUM(C2:C12)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>6</v>
       </c>
       <c r="C3" s="9">
         <v>3</v>
       </c>
-      <c r="D3" s="52">
-        <f>SUM(C3:C13)</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="63"/>
+      <c r="D3" s="48"/>
+    </row>
+    <row r="4" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="56" t="s">
+        <v>69</v>
+      </c>
       <c r="B4" s="9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="9">
-        <v>3</v>
-      </c>
-      <c r="D4" s="52"/>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="63"/>
+        <v>2</v>
+      </c>
+      <c r="D4" s="48"/>
+    </row>
+    <row r="5" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="56" t="s">
+        <v>69</v>
+      </c>
       <c r="B5" s="9" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C5" s="9">
         <v>2</v>
       </c>
-      <c r="D5" s="52"/>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="63"/>
+      <c r="D5" s="48"/>
+    </row>
+    <row r="6" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="56" t="s">
+        <v>69</v>
+      </c>
       <c r="B6" s="9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C6" s="9">
         <v>2</v>
       </c>
-      <c r="D6" s="52"/>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="63"/>
+      <c r="D6" s="48"/>
+    </row>
+    <row r="7" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="56" t="s">
+        <v>69</v>
+      </c>
       <c r="B7" s="9" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C7" s="9">
-        <v>2</v>
-      </c>
-      <c r="D7" s="52"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="63"/>
+        <v>3</v>
+      </c>
+      <c r="D7" s="48"/>
+    </row>
+    <row r="8" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="56" t="s">
+        <v>69</v>
+      </c>
       <c r="B8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="9">
         <v>4</v>
       </c>
-      <c r="C8" s="9">
-        <v>3</v>
-      </c>
-      <c r="D8" s="52"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="63"/>
+      <c r="D8" s="48"/>
+    </row>
+    <row r="9" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="56" t="s">
+        <v>69</v>
+      </c>
       <c r="B9" s="9" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="C9" s="9">
         <v>4</v>
       </c>
-      <c r="D9" s="52"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="63"/>
+      <c r="D9" s="48"/>
+    </row>
+    <row r="10" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="56" t="s">
+        <v>69</v>
+      </c>
       <c r="B10" s="9" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="C10" s="9">
         <v>4</v>
       </c>
-      <c r="D10" s="52"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="63"/>
+      <c r="D10" s="48"/>
+    </row>
+    <row r="11" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="56" t="s">
+        <v>69</v>
+      </c>
       <c r="B11" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11" s="9">
-        <v>4</v>
-      </c>
-      <c r="D11" s="52"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="63"/>
-      <c r="B12" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="9">
         <v>2</v>
       </c>
-      <c r="D12" s="52"/>
-    </row>
-    <row r="13" spans="1:4" ht="16.2" thickBot="1">
-      <c r="A13" s="64"/>
-      <c r="B13" s="18" t="s">
+      <c r="D11" s="48"/>
+    </row>
+    <row r="12" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C12" s="18">
         <v>1</v>
       </c>
-      <c r="D13" s="53"/>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="65" t="s">
-        <v>75</v>
-      </c>
-      <c r="B14" s="17" t="s">
+      <c r="D12" s="49"/>
+    </row>
+    <row r="13" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="57" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="17">
+      <c r="C13" s="17">
         <v>3</v>
       </c>
-      <c r="D14" s="51">
-        <f>SUM(C14:C24)</f>
+      <c r="D13" s="47">
+        <f>SUM(C13:C23)</f>
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="66"/>
+    <row r="14" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="57" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="9">
+        <v>3</v>
+      </c>
+      <c r="D14" s="48"/>
+    </row>
+    <row r="15" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="57" t="s">
+        <v>70</v>
+      </c>
       <c r="B15" s="9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C15" s="9">
-        <v>3</v>
-      </c>
-      <c r="D15" s="52"/>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="66"/>
+        <v>2</v>
+      </c>
+      <c r="D15" s="48"/>
+    </row>
+    <row r="16" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="57" t="s">
+        <v>70</v>
+      </c>
       <c r="B16" s="9" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C16" s="9">
         <v>2</v>
       </c>
-      <c r="D16" s="52"/>
-    </row>
-    <row r="17" spans="1:4" ht="31.2">
-      <c r="A17" s="66"/>
+      <c r="D16" s="48"/>
+    </row>
+    <row r="17" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="57" t="s">
+        <v>70</v>
+      </c>
       <c r="B17" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C17" s="9">
         <v>2</v>
       </c>
-      <c r="D17" s="52"/>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="66"/>
+      <c r="D17" s="48"/>
+    </row>
+    <row r="18" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="57" t="s">
+        <v>70</v>
+      </c>
       <c r="B18" s="9" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C18" s="9">
-        <v>2</v>
-      </c>
-      <c r="D18" s="52"/>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="66"/>
+        <v>3</v>
+      </c>
+      <c r="D18" s="48"/>
+    </row>
+    <row r="19" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="57" t="s">
+        <v>70</v>
+      </c>
       <c r="B19" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="9">
         <v>4</v>
       </c>
-      <c r="C19" s="9">
-        <v>3</v>
-      </c>
-      <c r="D19" s="52"/>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="66"/>
+      <c r="D19" s="48"/>
+    </row>
+    <row r="20" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="57" t="s">
+        <v>70</v>
+      </c>
       <c r="B20" s="9" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="C20" s="9">
         <v>4</v>
       </c>
-      <c r="D20" s="52"/>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="66"/>
+      <c r="D20" s="48"/>
+    </row>
+    <row r="21" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="57" t="s">
+        <v>70</v>
+      </c>
       <c r="B21" s="9" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="C21" s="9">
         <v>4</v>
       </c>
-      <c r="D21" s="52"/>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="66"/>
+      <c r="D21" s="48"/>
+    </row>
+    <row r="22" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="57" t="s">
+        <v>70</v>
+      </c>
       <c r="B22" s="9" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C22" s="9">
-        <v>4</v>
-      </c>
-      <c r="D22" s="52"/>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="66"/>
-      <c r="B23" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="9">
         <v>2</v>
       </c>
-      <c r="D23" s="52"/>
-    </row>
-    <row r="24" spans="1:4" ht="16.2" thickBot="1">
-      <c r="A24" s="67"/>
-      <c r="B24" s="18" t="s">
+      <c r="D22" s="48"/>
+    </row>
+    <row r="23" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="57" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="18">
+      <c r="C23" s="18">
         <v>1</v>
       </c>
-      <c r="D24" s="53"/>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="68" t="s">
-        <v>76</v>
-      </c>
-      <c r="B25" s="17" t="s">
+      <c r="D23" s="49"/>
+    </row>
+    <row r="24" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="58" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="17">
+      <c r="C24" s="17">
         <v>2</v>
       </c>
-      <c r="D25" s="51">
-        <f>SUM(C25:C36)</f>
+      <c r="D24" s="47">
+        <f>SUM(C24:C35)</f>
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="69"/>
+    <row r="25" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="58" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="9">
+        <v>2</v>
+      </c>
+      <c r="D25" s="48"/>
+    </row>
+    <row r="26" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="58" t="s">
+        <v>71</v>
+      </c>
       <c r="B26" s="9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C26" s="9">
         <v>2</v>
       </c>
-      <c r="D26" s="52"/>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="69"/>
+      <c r="D26" s="48"/>
+    </row>
+    <row r="27" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="58" t="s">
+        <v>71</v>
+      </c>
       <c r="B27" s="9" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C27" s="9">
         <v>2</v>
       </c>
-      <c r="D27" s="52"/>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="69"/>
+      <c r="D27" s="48"/>
+    </row>
+    <row r="28" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="58" t="s">
+        <v>71</v>
+      </c>
       <c r="B28" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C28" s="9">
-        <v>2</v>
-      </c>
-      <c r="D28" s="52"/>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="69"/>
+        <v>3</v>
+      </c>
+      <c r="D28" s="48"/>
+    </row>
+    <row r="29" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="58" t="s">
+        <v>71</v>
+      </c>
       <c r="B29" s="9" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C29" s="9">
         <v>3</v>
       </c>
-      <c r="D29" s="52"/>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="69"/>
+      <c r="D29" s="48"/>
+    </row>
+    <row r="30" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="58" t="s">
+        <v>71</v>
+      </c>
       <c r="B30" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="9">
         <v>4</v>
       </c>
-      <c r="C30" s="9">
-        <v>3</v>
-      </c>
-      <c r="D30" s="52"/>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="69"/>
+      <c r="D30" s="48"/>
+    </row>
+    <row r="31" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="58" t="s">
+        <v>71</v>
+      </c>
       <c r="B31" s="9" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="C31" s="9">
         <v>4</v>
       </c>
-      <c r="D31" s="52"/>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="69"/>
+      <c r="D31" s="48"/>
+    </row>
+    <row r="32" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="58" t="s">
+        <v>71</v>
+      </c>
       <c r="B32" s="9" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="C32" s="9">
         <v>4</v>
       </c>
-      <c r="D32" s="52"/>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="69"/>
+      <c r="D32" s="48"/>
+    </row>
+    <row r="33" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="58" t="s">
+        <v>71</v>
+      </c>
       <c r="B33" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C33" s="9">
-        <v>4</v>
-      </c>
-      <c r="D33" s="52"/>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="69"/>
+        <v>2</v>
+      </c>
+      <c r="D33" s="48"/>
+    </row>
+    <row r="34" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="58" t="s">
+        <v>71</v>
+      </c>
       <c r="B34" s="9" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C34" s="9">
+        <v>1</v>
+      </c>
+      <c r="D34" s="48"/>
+    </row>
+    <row r="35" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="58" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="18">
+        <v>1</v>
+      </c>
+      <c r="D35" s="49"/>
+    </row>
+    <row r="36" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="17">
+        <v>1</v>
+      </c>
+      <c r="D36" s="47">
+        <f>SUM(C36:C46)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="9">
+        <v>3</v>
+      </c>
+      <c r="D37" s="48"/>
+    </row>
+    <row r="38" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="9">
         <v>2</v>
       </c>
-      <c r="D34" s="52"/>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="69"/>
-      <c r="B35" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" s="9">
-        <v>1</v>
-      </c>
-      <c r="D35" s="52"/>
-    </row>
-    <row r="36" spans="1:4" ht="16.2" thickBot="1">
-      <c r="A36" s="70"/>
-      <c r="B36" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C36" s="18">
-        <v>1</v>
-      </c>
-      <c r="D36" s="53"/>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="48" t="s">
-        <v>77</v>
-      </c>
-      <c r="B37" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" s="17">
-        <v>1</v>
-      </c>
-      <c r="D37" s="51">
-        <f>SUM(C37:C47)</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="49"/>
-      <c r="B38" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C38" s="9">
-        <v>3</v>
-      </c>
-      <c r="D38" s="52"/>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="49"/>
+      <c r="D38" s="48"/>
+    </row>
+    <row r="39" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="59" t="s">
+        <v>72</v>
+      </c>
       <c r="B39" s="9" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C39" s="9">
         <v>2</v>
       </c>
-      <c r="D39" s="52"/>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="49"/>
+      <c r="D39" s="48"/>
+    </row>
+    <row r="40" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="59" t="s">
+        <v>72</v>
+      </c>
       <c r="B40" s="9" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C40" s="9">
-        <v>2</v>
-      </c>
-      <c r="D40" s="52"/>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="49"/>
+        <v>3</v>
+      </c>
+      <c r="D40" s="48"/>
+    </row>
+    <row r="41" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="59" t="s">
+        <v>72</v>
+      </c>
       <c r="B41" s="9" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C41" s="9">
         <v>3</v>
       </c>
-      <c r="D41" s="52"/>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="49"/>
+      <c r="D41" s="48"/>
+    </row>
+    <row r="42" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="59" t="s">
+        <v>72</v>
+      </c>
       <c r="B42" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="9">
         <v>4</v>
       </c>
-      <c r="C42" s="9">
-        <v>3</v>
-      </c>
-      <c r="D42" s="52"/>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="49"/>
+      <c r="D42" s="48"/>
+    </row>
+    <row r="43" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="59" t="s">
+        <v>72</v>
+      </c>
       <c r="B43" s="9" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="C43" s="9">
         <v>4</v>
       </c>
-      <c r="D43" s="52"/>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="49"/>
+      <c r="D43" s="48"/>
+    </row>
+    <row r="44" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="59" t="s">
+        <v>72</v>
+      </c>
       <c r="B44" s="9" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="C44" s="9">
-        <v>4</v>
-      </c>
-      <c r="D44" s="52"/>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="49"/>
+        <v>2</v>
+      </c>
+      <c r="D44" s="48"/>
+    </row>
+    <row r="45" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="59" t="s">
+        <v>72</v>
+      </c>
       <c r="B45" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C45" s="9">
         <v>2</v>
       </c>
-      <c r="D45" s="52"/>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="49"/>
-      <c r="B46" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C46" s="9">
+      <c r="D45" s="48"/>
+    </row>
+    <row r="46" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="B46" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C46" s="18">
+        <v>4</v>
+      </c>
+      <c r="D46" s="49"/>
+    </row>
+    <row r="47" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="60" t="s">
+        <v>73</v>
+      </c>
+      <c r="B47" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C47" s="17">
+        <v>4</v>
+      </c>
+      <c r="D47" s="47">
+        <f>SUM(C47:C56)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="60" t="s">
+        <v>73</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C48" s="9">
+        <v>3</v>
+      </c>
+      <c r="D48" s="48"/>
+    </row>
+    <row r="49" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="60" t="s">
+        <v>73</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C49" s="9">
         <v>2</v>
       </c>
-      <c r="D46" s="52"/>
-    </row>
-    <row r="47" spans="1:4" ht="16.2" thickBot="1">
-      <c r="A47" s="50"/>
-      <c r="B47" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C47" s="18">
-        <v>4</v>
-      </c>
-      <c r="D47" s="53"/>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="54" t="s">
-        <v>78</v>
-      </c>
-      <c r="B48" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C48" s="17">
-        <v>4</v>
-      </c>
-      <c r="D48" s="51">
-        <f>SUM(C48:C57)</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="55"/>
-      <c r="B49" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C49" s="9">
-        <v>3</v>
-      </c>
-      <c r="D49" s="52"/>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="55"/>
+      <c r="D49" s="48"/>
+    </row>
+    <row r="50" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="60" t="s">
+        <v>73</v>
+      </c>
       <c r="B50" s="9" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="C50" s="9">
         <v>2</v>
       </c>
-      <c r="D50" s="52"/>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="55"/>
+      <c r="D50" s="48"/>
+    </row>
+    <row r="51" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="60" t="s">
+        <v>73</v>
+      </c>
       <c r="B51" s="9" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C51" s="9">
+        <v>3</v>
+      </c>
+      <c r="D51" s="48"/>
+    </row>
+    <row r="52" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="60" t="s">
+        <v>73</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C52" s="9">
         <v>2</v>
       </c>
-      <c r="D51" s="52"/>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="55"/>
-      <c r="B52" s="9" t="s">
+      <c r="D52" s="48"/>
+    </row>
+    <row r="53" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="60" t="s">
+        <v>73</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" s="9">
         <v>4</v>
       </c>
-      <c r="C52" s="9">
-        <v>3</v>
-      </c>
-      <c r="D52" s="52"/>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="55"/>
-      <c r="B53" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C53" s="9">
-        <v>2</v>
-      </c>
-      <c r="D53" s="52"/>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="55"/>
+      <c r="D53" s="48"/>
+    </row>
+    <row r="54" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="60" t="s">
+        <v>73</v>
+      </c>
       <c r="B54" s="9" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="C54" s="9">
         <v>4</v>
       </c>
-      <c r="D54" s="52"/>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="55"/>
+      <c r="D54" s="48"/>
+    </row>
+    <row r="55" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="60" t="s">
+        <v>73</v>
+      </c>
       <c r="B55" s="9" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C55" s="9">
+        <v>3</v>
+      </c>
+      <c r="D55" s="48"/>
+    </row>
+    <row r="56" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="60" t="s">
+        <v>73</v>
+      </c>
+      <c r="B56" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C56" s="18">
+        <v>3</v>
+      </c>
+      <c r="D56" s="49"/>
+    </row>
+    <row r="57" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="B57" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C57" s="17">
         <v>4</v>
       </c>
-      <c r="D55" s="52"/>
-    </row>
-    <row r="56" spans="1:4" ht="31.2">
-      <c r="A56" s="55"/>
-      <c r="B56" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C56" s="9">
+      <c r="D57" s="48">
+        <f>SUM(C57:C65)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C58" s="9">
+        <v>4</v>
+      </c>
+      <c r="D58" s="48"/>
+    </row>
+    <row r="59" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C59" s="9">
         <v>3</v>
       </c>
-      <c r="D56" s="52"/>
-    </row>
-    <row r="57" spans="1:4" ht="16.2" thickBot="1">
-      <c r="A57" s="56"/>
-      <c r="B57" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C57" s="18">
-        <v>3</v>
-      </c>
-      <c r="D57" s="53"/>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="57" t="s">
-        <v>79</v>
-      </c>
-      <c r="B58" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C58" s="17">
-        <v>4</v>
-      </c>
-      <c r="D58" s="52">
-        <f>SUM(C58:C66)</f>
+      <c r="D59" s="48"/>
+    </row>
+    <row r="60" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="B60" s="9" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="58"/>
-      <c r="B59" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C59" s="9">
-        <v>4</v>
-      </c>
-      <c r="D59" s="52"/>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="58"/>
-      <c r="B60" s="9" t="s">
-        <v>29</v>
       </c>
       <c r="C60" s="9">
         <v>3</v>
       </c>
-      <c r="D60" s="52"/>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="58"/>
+      <c r="D60" s="48"/>
+    </row>
+    <row r="61" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="61" t="s">
+        <v>74</v>
+      </c>
       <c r="B61" s="9" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="C61" s="9">
-        <v>3</v>
-      </c>
-      <c r="D61" s="52"/>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="58"/>
+        <v>4</v>
+      </c>
+      <c r="D61" s="48"/>
+    </row>
+    <row r="62" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="61" t="s">
+        <v>74</v>
+      </c>
       <c r="B62" s="9" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C62" s="9">
         <v>4</v>
       </c>
-      <c r="D62" s="52"/>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="58"/>
+      <c r="D62" s="48"/>
+    </row>
+    <row r="63" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="61" t="s">
+        <v>74</v>
+      </c>
       <c r="B63" s="9" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="C63" s="9">
         <v>4</v>
       </c>
-      <c r="D63" s="52"/>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64" s="58"/>
+      <c r="D63" s="48"/>
+    </row>
+    <row r="64" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="61" t="s">
+        <v>74</v>
+      </c>
       <c r="B64" s="9" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C64" s="9">
-        <v>4</v>
-      </c>
-      <c r="D64" s="52"/>
-    </row>
-    <row r="65" spans="1:4">
-      <c r="A65" s="58"/>
-      <c r="B65" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C65" s="9">
         <v>2</v>
       </c>
-      <c r="D65" s="52"/>
-    </row>
-    <row r="66" spans="1:4" ht="16.2" thickBot="1">
-      <c r="A66" s="59"/>
-      <c r="B66" s="18" t="s">
+      <c r="D64" s="48"/>
+    </row>
+    <row r="65" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="B65" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C66" s="18">
+      <c r="C65" s="18">
         <v>2</v>
       </c>
-      <c r="D66" s="53"/>
-    </row>
+      <c r="D65" s="49"/>
+    </row>
+    <row r="66" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A25:A36"/>
-    <mergeCell ref="D25:D36"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A3:A13"/>
-    <mergeCell ref="D3:D13"/>
-    <mergeCell ref="A14:A24"/>
-    <mergeCell ref="D14:D24"/>
-    <mergeCell ref="A37:A47"/>
-    <mergeCell ref="D37:D47"/>
-    <mergeCell ref="A48:A57"/>
-    <mergeCell ref="D48:D57"/>
-    <mergeCell ref="A58:A66"/>
-    <mergeCell ref="D58:D66"/>
+  <mergeCells count="6">
+    <mergeCell ref="D36:D46"/>
+    <mergeCell ref="D47:D56"/>
+    <mergeCell ref="D57:D65"/>
+    <mergeCell ref="D24:D35"/>
+    <mergeCell ref="D2:D12"/>
+    <mergeCell ref="D13:D23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3062,179 +3066,184 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1926007A-6418-CC4B-9DC0-43BC3D9D373B}">
   <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="46.5" style="1" customWidth="1"/>
     <col min="2" max="4" width="17" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.69921875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.796875" customWidth="1"/>
-    <col min="7" max="7" width="10.796875" style="5"/>
+    <col min="5" max="5" width="9.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="71" t="s">
-        <v>81</v>
-      </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
+    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>40</v>
+      </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>40</v>
+    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9">
+        <f t="shared" ref="E2:E7" si="0">COUNTA(B2:D2)</f>
+        <v>1</v>
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9">
-        <f t="shared" ref="E3:E8" si="0">COUNTA(B3:D3)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C4" s="9"/>
+        <v>43</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>51</v>
+      </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>52</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="9"/>
+        <v>45</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>46</v>
+      </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>46</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" ht="15.6" customHeight="1">
+    <row r="8" spans="1:6" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" s="9"/>
+        <v>58</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>57</v>
+      </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9">
-        <f t="shared" si="0"/>
+        <f>COUNTA(C8:D8)</f>
         <v>1</v>
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>59</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="9">
-        <f>COUNTA(C9:D9)</f>
+        <f t="shared" ref="E9:E29" si="1">COUNTA(B9:D9)</f>
         <v>1</v>
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9">
-        <f t="shared" ref="E10:E30" si="1">COUNTA(B10:D10)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
@@ -3244,44 +3253,44 @@
       </c>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" s="9"/>
+        <v>59</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>64</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="C13" s="9"/>
       <c r="D13" s="9"/>
       <c r="E13" s="9">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
@@ -3291,12 +3300,12 @@
       </c>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -3306,12 +3315,12 @@
       </c>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
@@ -3321,49 +3330,51 @@
       </c>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
+        <v>42</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="E17" s="9">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>38</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="D18" s="9"/>
       <c r="E18" s="9">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9">
@@ -3372,99 +3383,97 @@
       </c>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D20" s="9"/>
+        <v>53</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>54</v>
+      </c>
       <c r="E20" s="9">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>47</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>56</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="D21" s="9"/>
       <c r="E21" s="9">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>55</v>
-      </c>
+      <c r="C22" s="9"/>
       <c r="D22" s="9"/>
       <c r="E22" s="9">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
+      <c r="C23" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>54</v>
+      </c>
       <c r="E23" s="9">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>56</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
       <c r="E24" s="9">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
@@ -3474,44 +3483,44 @@
       </c>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" s="9"/>
+        <v>52</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>67</v>
+      </c>
       <c r="D26" s="9"/>
       <c r="E26" s="9">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>71</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="C27" s="9"/>
       <c r="D27" s="9"/>
       <c r="E27" s="9">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
@@ -3521,415 +3530,395 @@
       </c>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9">
+    <row r="29" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="62" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="63"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="63">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="44"/>
+      <c r="B30" s="64"/>
+      <c r="C30" s="64"/>
+      <c r="D30" s="64"/>
+      <c r="E30" s="28"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="41">
-        <f>COUNTA(A3:A30)</f>
-        <v>28</v>
-      </c>
-      <c r="B31" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="C31" s="73"/>
-      <c r="D31" s="74"/>
-      <c r="E31" s="42">
-        <v>32</v>
-      </c>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="25"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="25"/>
-      <c r="B32" s="25"/>
+      <c r="B32" s="44"/>
       <c r="C32" s="25"/>
       <c r="D32" s="25"/>
       <c r="E32" s="25"/>
       <c r="F32" s="26"/>
-      <c r="G32" s="43"/>
+      <c r="G32" s="41"/>
       <c r="H32" s="26"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="25"/>
-      <c r="B33" s="46"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
       <c r="F33" s="25"/>
-      <c r="G33" s="75"/>
+      <c r="G33" s="50"/>
       <c r="H33" s="26"/>
     </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="25"/>
-      <c r="B34" s="27"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="42"/>
+      <c r="B34" s="33"/>
+      <c r="C34" s="33"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="33"/>
       <c r="F34" s="27"/>
-      <c r="G34" s="75"/>
+      <c r="G34" s="50"/>
       <c r="H34" s="26"/>
     </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="44"/>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="42"/>
       <c r="B35" s="33"/>
       <c r="C35" s="33"/>
       <c r="D35" s="33"/>
       <c r="E35" s="33"/>
       <c r="F35" s="33"/>
-      <c r="G35" s="43"/>
+      <c r="G35" s="41"/>
       <c r="H35" s="26"/>
     </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="44"/>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="42"/>
       <c r="B36" s="33"/>
       <c r="C36" s="33"/>
       <c r="D36" s="33"/>
       <c r="E36" s="33"/>
       <c r="F36" s="33"/>
-      <c r="G36" s="43"/>
+      <c r="G36" s="41"/>
       <c r="H36" s="26"/>
     </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="44"/>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="42"/>
       <c r="B37" s="33"/>
       <c r="C37" s="33"/>
       <c r="D37" s="33"/>
       <c r="E37" s="33"/>
       <c r="F37" s="33"/>
-      <c r="G37" s="43"/>
+      <c r="G37" s="41"/>
       <c r="H37" s="26"/>
     </row>
-    <row r="38" spans="1:8">
-      <c r="A38" s="44"/>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="42"/>
       <c r="B38" s="33"/>
       <c r="C38" s="33"/>
       <c r="D38" s="33"/>
       <c r="E38" s="33"/>
       <c r="F38" s="33"/>
-      <c r="G38" s="43"/>
+      <c r="G38" s="41"/>
       <c r="H38" s="26"/>
     </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="44"/>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="42"/>
       <c r="B39" s="33"/>
       <c r="C39" s="33"/>
       <c r="D39" s="33"/>
       <c r="E39" s="33"/>
       <c r="F39" s="33"/>
-      <c r="G39" s="43"/>
+      <c r="G39" s="41"/>
       <c r="H39" s="26"/>
     </row>
-    <row r="40" spans="1:8">
-      <c r="A40" s="44"/>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="42"/>
       <c r="B40" s="33"/>
       <c r="C40" s="33"/>
       <c r="D40" s="33"/>
       <c r="E40" s="33"/>
       <c r="F40" s="33"/>
-      <c r="G40" s="43"/>
+      <c r="G40" s="41"/>
       <c r="H40" s="26"/>
     </row>
-    <row r="41" spans="1:8">
-      <c r="A41" s="44"/>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="42"/>
       <c r="B41" s="33"/>
       <c r="C41" s="33"/>
       <c r="D41" s="33"/>
       <c r="E41" s="33"/>
       <c r="F41" s="33"/>
-      <c r="G41" s="43"/>
+      <c r="G41" s="41"/>
       <c r="H41" s="26"/>
     </row>
-    <row r="42" spans="1:8">
-      <c r="A42" s="44"/>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="42"/>
       <c r="B42" s="33"/>
       <c r="C42" s="33"/>
       <c r="D42" s="33"/>
       <c r="E42" s="33"/>
       <c r="F42" s="33"/>
-      <c r="G42" s="43"/>
+      <c r="G42" s="41"/>
       <c r="H42" s="26"/>
     </row>
-    <row r="43" spans="1:8">
-      <c r="A43" s="44"/>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="42"/>
       <c r="B43" s="33"/>
       <c r="C43" s="33"/>
       <c r="D43" s="33"/>
       <c r="E43" s="33"/>
       <c r="F43" s="33"/>
-      <c r="G43" s="43"/>
+      <c r="G43" s="41"/>
       <c r="H43" s="26"/>
     </row>
-    <row r="44" spans="1:8">
-      <c r="A44" s="44"/>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="42"/>
       <c r="B44" s="33"/>
       <c r="C44" s="33"/>
       <c r="D44" s="33"/>
       <c r="E44" s="33"/>
       <c r="F44" s="33"/>
-      <c r="G44" s="43"/>
+      <c r="G44" s="41"/>
       <c r="H44" s="26"/>
     </row>
-    <row r="45" spans="1:8">
-      <c r="A45" s="44"/>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="42"/>
       <c r="B45" s="33"/>
       <c r="C45" s="33"/>
       <c r="D45" s="33"/>
       <c r="E45" s="33"/>
       <c r="F45" s="33"/>
-      <c r="G45" s="43"/>
+      <c r="G45" s="41"/>
       <c r="H45" s="26"/>
     </row>
-    <row r="46" spans="1:8">
-      <c r="A46" s="44"/>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="42"/>
       <c r="B46" s="33"/>
       <c r="C46" s="33"/>
       <c r="D46" s="33"/>
       <c r="E46" s="33"/>
       <c r="F46" s="33"/>
-      <c r="G46" s="43"/>
+      <c r="G46" s="41"/>
       <c r="H46" s="26"/>
     </row>
-    <row r="47" spans="1:8">
-      <c r="A47" s="44"/>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="42"/>
       <c r="B47" s="33"/>
       <c r="C47" s="33"/>
       <c r="D47" s="33"/>
       <c r="E47" s="33"/>
       <c r="F47" s="33"/>
-      <c r="G47" s="43"/>
+      <c r="G47" s="41"/>
       <c r="H47" s="26"/>
     </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="44"/>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="42"/>
       <c r="B48" s="33"/>
       <c r="C48" s="33"/>
       <c r="D48" s="33"/>
       <c r="E48" s="33"/>
       <c r="F48" s="33"/>
-      <c r="G48" s="43"/>
+      <c r="G48" s="41"/>
       <c r="H48" s="26"/>
     </row>
-    <row r="49" spans="1:8">
-      <c r="A49" s="44"/>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="42"/>
       <c r="B49" s="33"/>
       <c r="C49" s="33"/>
       <c r="D49" s="33"/>
       <c r="E49" s="33"/>
       <c r="F49" s="33"/>
-      <c r="G49" s="43"/>
+      <c r="G49" s="41"/>
       <c r="H49" s="26"/>
     </row>
-    <row r="50" spans="1:8">
-      <c r="A50" s="44"/>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="42"/>
       <c r="B50" s="33"/>
       <c r="C50" s="33"/>
       <c r="D50" s="33"/>
       <c r="E50" s="33"/>
       <c r="F50" s="33"/>
-      <c r="G50" s="43"/>
+      <c r="G50" s="41"/>
       <c r="H50" s="26"/>
     </row>
-    <row r="51" spans="1:8">
-      <c r="A51" s="44"/>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="42"/>
       <c r="B51" s="33"/>
       <c r="C51" s="33"/>
       <c r="D51" s="33"/>
       <c r="E51" s="33"/>
       <c r="F51" s="33"/>
-      <c r="G51" s="43"/>
+      <c r="G51" s="41"/>
       <c r="H51" s="26"/>
     </row>
-    <row r="52" spans="1:8">
-      <c r="A52" s="44"/>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="42"/>
       <c r="B52" s="33"/>
       <c r="C52" s="33"/>
       <c r="D52" s="33"/>
       <c r="E52" s="33"/>
       <c r="F52" s="33"/>
-      <c r="G52" s="43"/>
+      <c r="G52" s="41"/>
       <c r="H52" s="26"/>
     </row>
-    <row r="53" spans="1:8">
-      <c r="A53" s="44"/>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="42"/>
       <c r="B53" s="33"/>
       <c r="C53" s="33"/>
       <c r="D53" s="33"/>
       <c r="E53" s="33"/>
       <c r="F53" s="33"/>
-      <c r="G53" s="43"/>
+      <c r="G53" s="41"/>
       <c r="H53" s="26"/>
     </row>
-    <row r="54" spans="1:8">
-      <c r="A54" s="44"/>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="42"/>
       <c r="B54" s="33"/>
       <c r="C54" s="33"/>
       <c r="D54" s="33"/>
       <c r="E54" s="33"/>
       <c r="F54" s="33"/>
-      <c r="G54" s="43"/>
+      <c r="G54" s="41"/>
       <c r="H54" s="26"/>
     </row>
-    <row r="55" spans="1:8">
-      <c r="A55" s="44"/>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="42"/>
       <c r="B55" s="33"/>
       <c r="C55" s="33"/>
       <c r="D55" s="33"/>
       <c r="E55" s="33"/>
       <c r="F55" s="33"/>
-      <c r="G55" s="43"/>
+      <c r="G55" s="41"/>
       <c r="H55" s="26"/>
     </row>
-    <row r="56" spans="1:8">
-      <c r="A56" s="44"/>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="42"/>
       <c r="B56" s="33"/>
       <c r="C56" s="33"/>
       <c r="D56" s="33"/>
       <c r="E56" s="33"/>
       <c r="F56" s="33"/>
-      <c r="G56" s="43"/>
+      <c r="G56" s="41"/>
       <c r="H56" s="26"/>
     </row>
-    <row r="57" spans="1:8">
-      <c r="A57" s="44"/>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="42"/>
       <c r="B57" s="33"/>
       <c r="C57" s="33"/>
       <c r="D57" s="33"/>
       <c r="E57" s="33"/>
       <c r="F57" s="33"/>
-      <c r="G57" s="43"/>
+      <c r="G57" s="41"/>
       <c r="H57" s="26"/>
     </row>
-    <row r="58" spans="1:8">
-      <c r="A58" s="44"/>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="42"/>
       <c r="B58" s="33"/>
       <c r="C58" s="33"/>
       <c r="D58" s="33"/>
       <c r="E58" s="33"/>
       <c r="F58" s="33"/>
-      <c r="G58" s="43"/>
+      <c r="G58" s="41"/>
       <c r="H58" s="26"/>
     </row>
-    <row r="59" spans="1:8">
-      <c r="A59" s="44"/>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="42"/>
       <c r="B59" s="33"/>
-      <c r="C59" s="33"/>
+      <c r="C59" s="25"/>
       <c r="D59" s="33"/>
       <c r="E59" s="33"/>
       <c r="F59" s="33"/>
-      <c r="G59" s="43"/>
+      <c r="G59" s="41"/>
       <c r="H59" s="26"/>
     </row>
-    <row r="60" spans="1:8">
-      <c r="A60" s="44"/>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="42"/>
       <c r="B60" s="33"/>
-      <c r="C60" s="25"/>
+      <c r="C60" s="33"/>
       <c r="D60" s="33"/>
       <c r="E60" s="33"/>
       <c r="F60" s="33"/>
-      <c r="G60" s="43"/>
+      <c r="G60" s="41"/>
       <c r="H60" s="26"/>
     </row>
-    <row r="61" spans="1:8">
-      <c r="A61" s="44"/>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="42"/>
       <c r="B61" s="33"/>
       <c r="C61" s="33"/>
       <c r="D61" s="33"/>
       <c r="E61" s="33"/>
       <c r="F61" s="33"/>
-      <c r="G61" s="43"/>
+      <c r="G61" s="41"/>
       <c r="H61" s="26"/>
     </row>
-    <row r="62" spans="1:8">
-      <c r="A62" s="44"/>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" s="42"/>
       <c r="B62" s="33"/>
       <c r="C62" s="33"/>
       <c r="D62" s="33"/>
       <c r="E62" s="33"/>
       <c r="F62" s="33"/>
-      <c r="G62" s="43"/>
+      <c r="G62" s="41"/>
       <c r="H62" s="26"/>
     </row>
-    <row r="63" spans="1:8">
-      <c r="A63" s="44"/>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="42"/>
       <c r="B63" s="33"/>
       <c r="C63" s="33"/>
       <c r="D63" s="33"/>
       <c r="E63" s="33"/>
       <c r="F63" s="33"/>
-      <c r="G63" s="43"/>
+      <c r="G63" s="41"/>
       <c r="H63" s="26"/>
     </row>
-    <row r="64" spans="1:8">
-      <c r="A64" s="44"/>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" s="43"/>
       <c r="B64" s="33"/>
       <c r="C64" s="33"/>
       <c r="D64" s="33"/>
       <c r="E64" s="33"/>
       <c r="F64" s="33"/>
-      <c r="G64" s="43"/>
+      <c r="G64" s="41"/>
       <c r="H64" s="26"/>
     </row>
-    <row r="65" spans="1:8">
-      <c r="A65" s="45"/>
-      <c r="B65" s="33"/>
-      <c r="C65" s="33"/>
-      <c r="D65" s="33"/>
-      <c r="E65" s="33"/>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" s="25"/>
+      <c r="B65" s="25"/>
+      <c r="C65" s="25"/>
+      <c r="D65" s="25"/>
+      <c r="E65" s="25"/>
       <c r="F65" s="34"/>
-      <c r="G65" s="43"/>
+      <c r="G65" s="41"/>
       <c r="H65" s="26"/>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="25"/>
       <c r="B66" s="25"/>
       <c r="C66" s="25"/>
       <c r="D66" s="25"/>
       <c r="E66" s="25"/>
       <c r="F66" s="26"/>
-      <c r="G66" s="43"/>
+      <c r="G66" s="41"/>
       <c r="H66" s="26"/>
     </row>
-    <row r="67" spans="1:8">
-      <c r="A67" s="25"/>
-      <c r="B67" s="25"/>
-      <c r="C67" s="25"/>
-      <c r="D67" s="25"/>
-      <c r="E67" s="25"/>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F67" s="26"/>
-      <c r="G67" s="43"/>
+      <c r="G67" s="41"/>
       <c r="H67" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="B31:D31"/>
+  <mergeCells count="2">
+    <mergeCell ref="B30:D30"/>
     <mergeCell ref="G33:G34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3940,238 +3929,242 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53966A10-ECE2-1349-837C-E1D3F35DE40D}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="92" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:XFD29"/>
+    <sheetView zoomScale="92" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="7" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="1"/>
-      <c r="B1" s="71" t="s">
-        <v>89</v>
-      </c>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="77" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1"/>
-      <c r="B2" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="G2" s="77"/>
-    </row>
-    <row r="3" spans="1:7">
+    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="53" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="45" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="15"/>
+      <c r="G2" s="32">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15" t="s">
-        <v>90</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="15"/>
       <c r="D3" s="15"/>
       <c r="E3" s="15" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="F3" s="15"/>
       <c r="G3" s="32">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="35" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15" t="s">
-        <v>90</v>
-      </c>
+      <c r="D4" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="32">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15" t="s">
-        <v>90</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="15"/>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="32">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="D6" s="15"/>
+        <v>83</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15" t="s">
+        <v>81</v>
+      </c>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
       <c r="G6" s="32">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="C7" s="15"/>
+        <v>84</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15" t="s">
+        <v>81</v>
+      </c>
       <c r="D7" s="15" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
       <c r="G7" s="32">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="35" t="s">
-        <v>93</v>
-      </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>90</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="32">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="35" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="C9" s="15"/>
+        <v>85</v>
+      </c>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15" t="s">
+        <v>81</v>
+      </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
       <c r="G9" s="32">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="35" t="s">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="B10" s="15"/>
-      <c r="C10" s="15" t="s">
-        <v>90</v>
-      </c>
+      <c r="C10" s="15"/>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
       <c r="G10" s="32">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.6" customHeight="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="35" t="s">
-        <v>66</v>
-      </c>
-      <c r="B11" s="15"/>
+        <v>59</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>81</v>
+      </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
       <c r="G11" s="32">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>90</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="B12" s="15"/>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
+      <c r="E12" s="15" t="s">
+        <v>81</v>
+      </c>
       <c r="F12" s="15"/>
       <c r="G12" s="32">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="35" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
+      <c r="C13" s="15" t="s">
+        <v>81</v>
+      </c>
       <c r="D13" s="15"/>
-      <c r="E13" s="15" t="s">
-        <v>90</v>
-      </c>
+      <c r="E13" s="15"/>
       <c r="F13" s="15"/>
       <c r="G13" s="32">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="35" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B14" s="15"/>
-      <c r="C14" s="15" t="s">
-        <v>90</v>
-      </c>
+      <c r="C14" s="15"/>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
       <c r="G14" s="32">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="35" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
@@ -4179,70 +4172,70 @@
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
       <c r="G15" s="32">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="35" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
+      <c r="F16" s="15" t="s">
+        <v>81</v>
+      </c>
       <c r="G16" s="32">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="35" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
       <c r="F17" s="15" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="G17" s="32">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="35" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
       <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
+      <c r="C18" s="15" t="s">
+        <v>81</v>
+      </c>
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
-      <c r="F18" s="15" t="s">
-        <v>90</v>
-      </c>
+      <c r="F18" s="15"/>
       <c r="G18" s="32">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="35" t="s">
-        <v>47</v>
+        <v>87</v>
       </c>
       <c r="B19" s="15"/>
-      <c r="C19" s="15" t="s">
-        <v>90</v>
-      </c>
+      <c r="C19" s="15"/>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
       <c r="G19" s="32">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="35" t="s">
-        <v>96</v>
+        <v>39</v>
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
@@ -4250,12 +4243,12 @@
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
       <c r="G20" s="32">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="35" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
@@ -4263,194 +4256,221 @@
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
       <c r="G21" s="32">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="35" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
+      <c r="E22" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>81</v>
+      </c>
       <c r="G22" s="32">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="35" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="F23" s="15" t="s">
-        <v>90</v>
-      </c>
+      <c r="C23" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
       <c r="G23" s="32">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="35" t="s">
-        <v>97</v>
+        <v>51</v>
       </c>
       <c r="B24" s="15"/>
       <c r="C24" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>90</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="D24" s="15"/>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
       <c r="G24" s="32">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="35" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B25" s="15"/>
       <c r="C25" s="15" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D25" s="15"/>
       <c r="E25" s="15"/>
       <c r="F25" s="15"/>
       <c r="G25" s="32">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="35" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="B26" s="15"/>
-      <c r="C26" s="15" t="s">
-        <v>90</v>
-      </c>
+      <c r="C26" s="15"/>
       <c r="D26" s="15"/>
       <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
+      <c r="F26" s="15" t="s">
+        <v>81</v>
+      </c>
       <c r="G26" s="32">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="35" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="15" t="s">
+        <v>81</v>
+      </c>
       <c r="E27" s="15"/>
-      <c r="F27" s="15" t="s">
-        <v>90</v>
-      </c>
+      <c r="F27" s="15"/>
       <c r="G27" s="32">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="35" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B28" s="15"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="15" t="s">
-        <v>90</v>
-      </c>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
       <c r="G28" s="32">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="B29" s="15"/>
+        <v>50</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>81</v>
+      </c>
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>
       <c r="E29" s="15"/>
       <c r="F29" s="15"/>
       <c r="G29" s="32">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="C30" s="15"/>
+        <v>48</v>
+      </c>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15" t="s">
+        <v>81</v>
+      </c>
       <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
+      <c r="E30" s="15" t="s">
+        <v>81</v>
+      </c>
       <c r="F30" s="15"/>
       <c r="G30" s="32">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="35" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B31" s="15"/>
-      <c r="C31" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15" t="s">
-        <v>90</v>
-      </c>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E31" s="15"/>
       <c r="F31" s="15"/>
       <c r="G31" s="32">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" ht="17" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED37D482-83EB-714D-B143-55F3284911A1}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="51" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="51" t="s">
         <v>90</v>
       </c>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="32">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="35" t="s">
-        <v>38</v>
-      </c>
-      <c r="B33" s="36"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="36"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="32">
-        <v>4</v>
+      <c r="C1" s="52" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="52" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5">
+        <v>7</v>
+      </c>
+      <c r="C2" s="65">
+        <v>8</v>
+      </c>
+      <c r="D2" s="65">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="G1:G2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
+ Implemented hard constraints functions + Modified functions to include parameter type
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreea/Desktop/20-21/1er Cuatrimestre/IC/Sebastián/Genetic_Timetable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3685C6F7-4A6C-B74B-9A11-02B06C381E24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC66BD2-9E5E-0742-ACA9-F2F0FB9CA4C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{BC545386-80F0-1D4E-9D05-34C34264D497}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{BC545386-80F0-1D4E-9D05-34C34264D497}"/>
   </bookViews>
   <sheets>
     <sheet name="course_hours" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="91">
   <si>
     <t>Inglés</t>
   </si>
@@ -304,6 +304,12 @@
   </si>
   <si>
     <t>Total horas/clase semanales</t>
+  </si>
+  <si>
+    <t>Cursos</t>
+  </si>
+  <si>
+    <t>1ESO, 2ESO, 3ESO, 4ESO, 1BATX, 2BATX</t>
   </si>
 </sst>
 </file>
@@ -548,7 +554,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -638,9 +644,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -674,9 +677,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -690,6 +690,9 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1006,20 +1009,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63029257-91CB-DE40-9386-1B96221C5B2F}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:D66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.33203125" style="34" customWidth="1"/>
-    <col min="2" max="4" width="35.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" style="33" customWidth="1"/>
+    <col min="2" max="2" width="52.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="32" t="s">
         <v>86</v>
       </c>
       <c r="B1" s="12" t="s">
@@ -1033,7 +1041,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="34" t="s">
         <v>62</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -1042,13 +1050,13 @@
       <c r="C2" s="5">
         <v>3</v>
       </c>
-      <c r="D2" s="45">
+      <c r="D2" s="43">
         <f>SUM(C2:C12)</f>
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="34" t="s">
         <v>62</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -1057,10 +1065,10 @@
       <c r="C3" s="5">
         <v>3</v>
       </c>
-      <c r="D3" s="45"/>
+      <c r="D3" s="43"/>
     </row>
     <row r="4" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="34" t="s">
         <v>62</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -1069,10 +1077,10 @@
       <c r="C4" s="5">
         <v>2</v>
       </c>
-      <c r="D4" s="45"/>
+      <c r="D4" s="43"/>
     </row>
     <row r="5" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="34" t="s">
         <v>62</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -1081,10 +1089,10 @@
       <c r="C5" s="5">
         <v>2</v>
       </c>
-      <c r="D5" s="45"/>
+      <c r="D5" s="43"/>
     </row>
     <row r="6" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="34" t="s">
         <v>62</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -1093,10 +1101,10 @@
       <c r="C6" s="5">
         <v>2</v>
       </c>
-      <c r="D6" s="45"/>
+      <c r="D6" s="43"/>
     </row>
     <row r="7" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="34" t="s">
         <v>62</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -1105,10 +1113,10 @@
       <c r="C7" s="5">
         <v>3</v>
       </c>
-      <c r="D7" s="45"/>
+      <c r="D7" s="43"/>
     </row>
     <row r="8" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="34" t="s">
         <v>62</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -1117,10 +1125,10 @@
       <c r="C8" s="5">
         <v>4</v>
       </c>
-      <c r="D8" s="45"/>
+      <c r="D8" s="43"/>
     </row>
     <row r="9" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="34" t="s">
         <v>62</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -1129,10 +1137,10 @@
       <c r="C9" s="5">
         <v>4</v>
       </c>
-      <c r="D9" s="45"/>
+      <c r="D9" s="43"/>
     </row>
     <row r="10" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="34" t="s">
         <v>62</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -1141,10 +1149,10 @@
       <c r="C10" s="5">
         <v>4</v>
       </c>
-      <c r="D10" s="45"/>
+      <c r="D10" s="43"/>
     </row>
     <row r="11" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="34" t="s">
         <v>62</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -1153,10 +1161,10 @@
       <c r="C11" s="5">
         <v>2</v>
       </c>
-      <c r="D11" s="45"/>
+      <c r="D11" s="43"/>
     </row>
     <row r="12" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="34" t="s">
         <v>62</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -1165,10 +1173,10 @@
       <c r="C12" s="8">
         <v>1</v>
       </c>
-      <c r="D12" s="46"/>
+      <c r="D12" s="44"/>
     </row>
     <row r="13" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="35" t="s">
         <v>63</v>
       </c>
       <c r="B13" s="7" t="s">
@@ -1177,13 +1185,13 @@
       <c r="C13" s="7">
         <v>3</v>
       </c>
-      <c r="D13" s="44">
+      <c r="D13" s="42">
         <f>SUM(C13:C23)</f>
         <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="35" t="s">
         <v>63</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -1192,10 +1200,10 @@
       <c r="C14" s="5">
         <v>3</v>
       </c>
-      <c r="D14" s="45"/>
+      <c r="D14" s="43"/>
     </row>
     <row r="15" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="35" t="s">
         <v>63</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -1204,10 +1212,10 @@
       <c r="C15" s="5">
         <v>2</v>
       </c>
-      <c r="D15" s="45"/>
+      <c r="D15" s="43"/>
     </row>
     <row r="16" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="35" t="s">
         <v>63</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -1216,10 +1224,10 @@
       <c r="C16" s="5">
         <v>2</v>
       </c>
-      <c r="D16" s="45"/>
+      <c r="D16" s="43"/>
     </row>
     <row r="17" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="35" t="s">
         <v>63</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -1228,10 +1236,10 @@
       <c r="C17" s="5">
         <v>2</v>
       </c>
-      <c r="D17" s="45"/>
+      <c r="D17" s="43"/>
     </row>
     <row r="18" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="36" t="s">
+      <c r="A18" s="35" t="s">
         <v>63</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -1240,10 +1248,10 @@
       <c r="C18" s="5">
         <v>3</v>
       </c>
-      <c r="D18" s="45"/>
+      <c r="D18" s="43"/>
     </row>
     <row r="19" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="35" t="s">
         <v>63</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -1252,10 +1260,10 @@
       <c r="C19" s="5">
         <v>4</v>
       </c>
-      <c r="D19" s="45"/>
+      <c r="D19" s="43"/>
     </row>
     <row r="20" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="36" t="s">
+      <c r="A20" s="35" t="s">
         <v>63</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -1264,10 +1272,10 @@
       <c r="C20" s="5">
         <v>4</v>
       </c>
-      <c r="D20" s="45"/>
+      <c r="D20" s="43"/>
     </row>
     <row r="21" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="36" t="s">
+      <c r="A21" s="35" t="s">
         <v>63</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -1276,10 +1284,10 @@
       <c r="C21" s="5">
         <v>4</v>
       </c>
-      <c r="D21" s="45"/>
+      <c r="D21" s="43"/>
     </row>
     <row r="22" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="36" t="s">
+      <c r="A22" s="35" t="s">
         <v>63</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -1288,10 +1296,10 @@
       <c r="C22" s="5">
         <v>2</v>
       </c>
-      <c r="D22" s="45"/>
+      <c r="D22" s="43"/>
     </row>
     <row r="23" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="36" t="s">
+      <c r="A23" s="35" t="s">
         <v>63</v>
       </c>
       <c r="B23" s="8" t="s">
@@ -1300,10 +1308,10 @@
       <c r="C23" s="8">
         <v>1</v>
       </c>
-      <c r="D23" s="46"/>
+      <c r="D23" s="44"/>
     </row>
     <row r="24" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="37" t="s">
+      <c r="A24" s="36" t="s">
         <v>64</v>
       </c>
       <c r="B24" s="7" t="s">
@@ -1312,13 +1320,13 @@
       <c r="C24" s="7">
         <v>2</v>
       </c>
-      <c r="D24" s="44">
+      <c r="D24" s="42">
         <f>SUM(C24:C35)</f>
         <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="37" t="s">
+      <c r="A25" s="36" t="s">
         <v>64</v>
       </c>
       <c r="B25" s="5" t="s">
@@ -1327,10 +1335,10 @@
       <c r="C25" s="5">
         <v>2</v>
       </c>
-      <c r="D25" s="45"/>
+      <c r="D25" s="43"/>
     </row>
     <row r="26" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="37" t="s">
+      <c r="A26" s="36" t="s">
         <v>64</v>
       </c>
       <c r="B26" s="5" t="s">
@@ -1339,10 +1347,10 @@
       <c r="C26" s="5">
         <v>2</v>
       </c>
-      <c r="D26" s="45"/>
+      <c r="D26" s="43"/>
     </row>
     <row r="27" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="36" t="s">
         <v>64</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -1351,10 +1359,10 @@
       <c r="C27" s="5">
         <v>2</v>
       </c>
-      <c r="D27" s="45"/>
+      <c r="D27" s="43"/>
     </row>
     <row r="28" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="36" t="s">
         <v>64</v>
       </c>
       <c r="B28" s="5" t="s">
@@ -1363,10 +1371,10 @@
       <c r="C28" s="5">
         <v>3</v>
       </c>
-      <c r="D28" s="45"/>
+      <c r="D28" s="43"/>
     </row>
     <row r="29" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="36" t="s">
         <v>64</v>
       </c>
       <c r="B29" s="5" t="s">
@@ -1375,10 +1383,10 @@
       <c r="C29" s="5">
         <v>3</v>
       </c>
-      <c r="D29" s="45"/>
+      <c r="D29" s="43"/>
     </row>
     <row r="30" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="37" t="s">
+      <c r="A30" s="36" t="s">
         <v>64</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -1387,10 +1395,10 @@
       <c r="C30" s="5">
         <v>4</v>
       </c>
-      <c r="D30" s="45"/>
+      <c r="D30" s="43"/>
     </row>
     <row r="31" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="37" t="s">
+      <c r="A31" s="36" t="s">
         <v>64</v>
       </c>
       <c r="B31" s="5" t="s">
@@ -1399,10 +1407,10 @@
       <c r="C31" s="5">
         <v>4</v>
       </c>
-      <c r="D31" s="45"/>
+      <c r="D31" s="43"/>
     </row>
     <row r="32" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="37" t="s">
+      <c r="A32" s="36" t="s">
         <v>64</v>
       </c>
       <c r="B32" s="5" t="s">
@@ -1411,10 +1419,10 @@
       <c r="C32" s="5">
         <v>4</v>
       </c>
-      <c r="D32" s="45"/>
+      <c r="D32" s="43"/>
     </row>
     <row r="33" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="36" t="s">
         <v>64</v>
       </c>
       <c r="B33" s="5" t="s">
@@ -1423,10 +1431,10 @@
       <c r="C33" s="5">
         <v>2</v>
       </c>
-      <c r="D33" s="45"/>
+      <c r="D33" s="43"/>
     </row>
     <row r="34" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="37" t="s">
+      <c r="A34" s="36" t="s">
         <v>64</v>
       </c>
       <c r="B34" s="5" t="s">
@@ -1435,10 +1443,10 @@
       <c r="C34" s="5">
         <v>1</v>
       </c>
-      <c r="D34" s="45"/>
+      <c r="D34" s="43"/>
     </row>
     <row r="35" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="37" t="s">
+      <c r="A35" s="36" t="s">
         <v>64</v>
       </c>
       <c r="B35" s="8" t="s">
@@ -1447,10 +1455,10 @@
       <c r="C35" s="8">
         <v>1</v>
       </c>
-      <c r="D35" s="46"/>
+      <c r="D35" s="44"/>
     </row>
     <row r="36" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="38" t="s">
+      <c r="A36" s="37" t="s">
         <v>65</v>
       </c>
       <c r="B36" s="7" t="s">
@@ -1459,13 +1467,13 @@
       <c r="C36" s="7">
         <v>1</v>
       </c>
-      <c r="D36" s="44">
+      <c r="D36" s="42">
         <f>SUM(C36:C46)</f>
         <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="38" t="s">
+      <c r="A37" s="37" t="s">
         <v>65</v>
       </c>
       <c r="B37" s="5" t="s">
@@ -1474,10 +1482,10 @@
       <c r="C37" s="5">
         <v>3</v>
       </c>
-      <c r="D37" s="45"/>
+      <c r="D37" s="43"/>
     </row>
     <row r="38" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="38" t="s">
+      <c r="A38" s="37" t="s">
         <v>65</v>
       </c>
       <c r="B38" s="5" t="s">
@@ -1486,10 +1494,10 @@
       <c r="C38" s="5">
         <v>2</v>
       </c>
-      <c r="D38" s="45"/>
+      <c r="D38" s="43"/>
     </row>
     <row r="39" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="38" t="s">
+      <c r="A39" s="37" t="s">
         <v>65</v>
       </c>
       <c r="B39" s="5" t="s">
@@ -1498,10 +1506,10 @@
       <c r="C39" s="5">
         <v>2</v>
       </c>
-      <c r="D39" s="45"/>
+      <c r="D39" s="43"/>
     </row>
     <row r="40" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="38" t="s">
+      <c r="A40" s="37" t="s">
         <v>65</v>
       </c>
       <c r="B40" s="5" t="s">
@@ -1510,10 +1518,10 @@
       <c r="C40" s="5">
         <v>3</v>
       </c>
-      <c r="D40" s="45"/>
+      <c r="D40" s="43"/>
     </row>
     <row r="41" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="38" t="s">
+      <c r="A41" s="37" t="s">
         <v>65</v>
       </c>
       <c r="B41" s="5" t="s">
@@ -1522,10 +1530,10 @@
       <c r="C41" s="5">
         <v>3</v>
       </c>
-      <c r="D41" s="45"/>
+      <c r="D41" s="43"/>
     </row>
     <row r="42" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="38" t="s">
+      <c r="A42" s="37" t="s">
         <v>65</v>
       </c>
       <c r="B42" s="5" t="s">
@@ -1534,10 +1542,10 @@
       <c r="C42" s="5">
         <v>4</v>
       </c>
-      <c r="D42" s="45"/>
+      <c r="D42" s="43"/>
     </row>
     <row r="43" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="38" t="s">
+      <c r="A43" s="37" t="s">
         <v>65</v>
       </c>
       <c r="B43" s="5" t="s">
@@ -1546,10 +1554,10 @@
       <c r="C43" s="5">
         <v>4</v>
       </c>
-      <c r="D43" s="45"/>
+      <c r="D43" s="43"/>
     </row>
     <row r="44" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="38" t="s">
+      <c r="A44" s="37" t="s">
         <v>65</v>
       </c>
       <c r="B44" s="5" t="s">
@@ -1558,10 +1566,10 @@
       <c r="C44" s="5">
         <v>2</v>
       </c>
-      <c r="D44" s="45"/>
+      <c r="D44" s="43"/>
     </row>
     <row r="45" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="38" t="s">
+      <c r="A45" s="37" t="s">
         <v>65</v>
       </c>
       <c r="B45" s="5" t="s">
@@ -1570,10 +1578,10 @@
       <c r="C45" s="5">
         <v>2</v>
       </c>
-      <c r="D45" s="45"/>
+      <c r="D45" s="43"/>
     </row>
     <row r="46" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="38" t="s">
+      <c r="A46" s="37" t="s">
         <v>65</v>
       </c>
       <c r="B46" s="8" t="s">
@@ -1582,10 +1590,10 @@
       <c r="C46" s="8">
         <v>4</v>
       </c>
-      <c r="D46" s="46"/>
+      <c r="D46" s="44"/>
     </row>
     <row r="47" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="39" t="s">
+      <c r="A47" s="38" t="s">
         <v>66</v>
       </c>
       <c r="B47" s="7" t="s">
@@ -1594,13 +1602,13 @@
       <c r="C47" s="7">
         <v>4</v>
       </c>
-      <c r="D47" s="44">
+      <c r="D47" s="42">
         <f>SUM(C47:C56)</f>
         <v>30</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="39" t="s">
+      <c r="A48" s="38" t="s">
         <v>66</v>
       </c>
       <c r="B48" s="5" t="s">
@@ -1609,10 +1617,10 @@
       <c r="C48" s="5">
         <v>3</v>
       </c>
-      <c r="D48" s="45"/>
+      <c r="D48" s="43"/>
     </row>
     <row r="49" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="39" t="s">
+      <c r="A49" s="38" t="s">
         <v>66</v>
       </c>
       <c r="B49" s="5" t="s">
@@ -1621,10 +1629,10 @@
       <c r="C49" s="5">
         <v>2</v>
       </c>
-      <c r="D49" s="45"/>
+      <c r="D49" s="43"/>
     </row>
     <row r="50" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="39" t="s">
+      <c r="A50" s="38" t="s">
         <v>66</v>
       </c>
       <c r="B50" s="5" t="s">
@@ -1633,10 +1641,10 @@
       <c r="C50" s="5">
         <v>2</v>
       </c>
-      <c r="D50" s="45"/>
+      <c r="D50" s="43"/>
     </row>
     <row r="51" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="39" t="s">
+      <c r="A51" s="38" t="s">
         <v>66</v>
       </c>
       <c r="B51" s="5" t="s">
@@ -1645,10 +1653,10 @@
       <c r="C51" s="5">
         <v>3</v>
       </c>
-      <c r="D51" s="45"/>
+      <c r="D51" s="43"/>
     </row>
     <row r="52" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="39" t="s">
+      <c r="A52" s="38" t="s">
         <v>66</v>
       </c>
       <c r="B52" s="5" t="s">
@@ -1657,10 +1665,10 @@
       <c r="C52" s="5">
         <v>2</v>
       </c>
-      <c r="D52" s="45"/>
+      <c r="D52" s="43"/>
     </row>
     <row r="53" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="39" t="s">
+      <c r="A53" s="38" t="s">
         <v>66</v>
       </c>
       <c r="B53" s="5" t="s">
@@ -1669,10 +1677,10 @@
       <c r="C53" s="5">
         <v>4</v>
       </c>
-      <c r="D53" s="45"/>
+      <c r="D53" s="43"/>
     </row>
     <row r="54" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="39" t="s">
+      <c r="A54" s="38" t="s">
         <v>66</v>
       </c>
       <c r="B54" s="5" t="s">
@@ -1681,10 +1689,10 @@
       <c r="C54" s="5">
         <v>4</v>
       </c>
-      <c r="D54" s="45"/>
+      <c r="D54" s="43"/>
     </row>
     <row r="55" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="39" t="s">
+      <c r="A55" s="38" t="s">
         <v>66</v>
       </c>
       <c r="B55" s="5" t="s">
@@ -1693,10 +1701,10 @@
       <c r="C55" s="5">
         <v>3</v>
       </c>
-      <c r="D55" s="45"/>
+      <c r="D55" s="43"/>
     </row>
     <row r="56" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="39" t="s">
+      <c r="A56" s="38" t="s">
         <v>66</v>
       </c>
       <c r="B56" s="8" t="s">
@@ -1705,10 +1713,10 @@
       <c r="C56" s="8">
         <v>3</v>
       </c>
-      <c r="D56" s="46"/>
+      <c r="D56" s="44"/>
     </row>
     <row r="57" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="40" t="s">
+      <c r="A57" s="39" t="s">
         <v>67</v>
       </c>
       <c r="B57" s="7" t="s">
@@ -1717,13 +1725,13 @@
       <c r="C57" s="7">
         <v>4</v>
       </c>
-      <c r="D57" s="45">
+      <c r="D57" s="43">
         <f>SUM(C57:C65)</f>
         <v>30</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="40" t="s">
+      <c r="A58" s="39" t="s">
         <v>67</v>
       </c>
       <c r="B58" s="5" t="s">
@@ -1732,10 +1740,10 @@
       <c r="C58" s="5">
         <v>4</v>
       </c>
-      <c r="D58" s="45"/>
+      <c r="D58" s="43"/>
     </row>
     <row r="59" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="40" t="s">
+      <c r="A59" s="39" t="s">
         <v>67</v>
       </c>
       <c r="B59" s="5" t="s">
@@ -1744,10 +1752,10 @@
       <c r="C59" s="5">
         <v>3</v>
       </c>
-      <c r="D59" s="45"/>
+      <c r="D59" s="43"/>
     </row>
     <row r="60" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="40" t="s">
+      <c r="A60" s="39" t="s">
         <v>67</v>
       </c>
       <c r="B60" s="5" t="s">
@@ -1756,10 +1764,10 @@
       <c r="C60" s="5">
         <v>3</v>
       </c>
-      <c r="D60" s="45"/>
+      <c r="D60" s="43"/>
     </row>
     <row r="61" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="40" t="s">
+      <c r="A61" s="39" t="s">
         <v>67</v>
       </c>
       <c r="B61" s="5" t="s">
@@ -1768,10 +1776,10 @@
       <c r="C61" s="5">
         <v>4</v>
       </c>
-      <c r="D61" s="45"/>
+      <c r="D61" s="43"/>
     </row>
     <row r="62" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="40" t="s">
+      <c r="A62" s="39" t="s">
         <v>67</v>
       </c>
       <c r="B62" s="5" t="s">
@@ -1780,10 +1788,10 @@
       <c r="C62" s="5">
         <v>4</v>
       </c>
-      <c r="D62" s="45"/>
+      <c r="D62" s="43"/>
     </row>
     <row r="63" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="40" t="s">
+      <c r="A63" s="39" t="s">
         <v>67</v>
       </c>
       <c r="B63" s="5" t="s">
@@ -1792,10 +1800,10 @@
       <c r="C63" s="5">
         <v>4</v>
       </c>
-      <c r="D63" s="45"/>
+      <c r="D63" s="43"/>
     </row>
     <row r="64" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="40" t="s">
+      <c r="A64" s="39" t="s">
         <v>67</v>
       </c>
       <c r="B64" s="5" t="s">
@@ -1804,10 +1812,10 @@
       <c r="C64" s="5">
         <v>2</v>
       </c>
-      <c r="D64" s="45"/>
+      <c r="D64" s="43"/>
     </row>
     <row r="65" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="40" t="s">
+      <c r="A65" s="39" t="s">
         <v>67</v>
       </c>
       <c r="B65" s="8" t="s">
@@ -1816,7 +1824,7 @@
       <c r="C65" s="8">
         <v>2</v>
       </c>
-      <c r="D65" s="46"/>
+      <c r="D65" s="44"/>
     </row>
     <row r="66" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -1829,6 +1837,7 @@
     <mergeCell ref="D13:D23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="70" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2301,15 +2310,15 @@
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="41" t="s">
+      <c r="A29" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="42" t="s">
+      <c r="B29" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="42"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="42">
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -2317,9 +2326,9 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="28"/>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
       <c r="E30" s="17"/>
       <c r="F30" s="1"/>
     </row>
@@ -2348,7 +2357,7 @@
       <c r="D33" s="16"/>
       <c r="E33" s="16"/>
       <c r="F33" s="14"/>
-      <c r="G33" s="48"/>
+      <c r="G33" s="46"/>
       <c r="H33" s="15"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -2358,7 +2367,7 @@
       <c r="D34" s="20"/>
       <c r="E34" s="20"/>
       <c r="F34" s="16"/>
-      <c r="G34" s="48"/>
+      <c r="G34" s="46"/>
       <c r="H34" s="15"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -2692,6 +2701,7 @@
     <mergeCell ref="G33:G34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2709,7 +2719,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
         <v>85</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -3199,48 +3209,60 @@
     <row r="33" ht="17" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED37D482-83EB-714D-B143-55F3284911A1}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="4" width="10.83203125" style="2"/>
+    <col min="5" max="5" width="39.1640625" style="2" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
         <v>81</v>
       </c>
       <c r="B1" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="30" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="30" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>5</v>
       </c>
       <c r="B2" s="2">
         <v>7</v>
       </c>
-      <c r="C2" s="43">
+      <c r="C2" s="47">
         <v>8</v>
       </c>
-      <c r="D2" s="43">
+      <c r="D2" s="47">
         <v>15</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Dejar solo un Teacher por Class
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreea/Desktop/20-21/1er Cuatrimestre/IC/Sebastián/Genetic_Timetable/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\5-MUSI\Inteligencia Computacional\Timetable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC66BD2-9E5E-0742-ACA9-F2F0FB9CA4C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA78AA5A-55C6-4718-A8BB-C5EFC6AC36CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{BC545386-80F0-1D4E-9D05-34C34264D497}"/>
+    <workbookView xWindow="-28920" yWindow="-12660" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{BC545386-80F0-1D4E-9D05-34C34264D497}"/>
   </bookViews>
   <sheets>
     <sheet name="course_hours" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="88">
   <si>
     <t>Inglés</t>
   </si>
@@ -123,12 +123,6 @@
     <t>Profesor 1</t>
   </si>
   <si>
-    <t>Profesor 2</t>
-  </si>
-  <si>
-    <t>Profesor 3</t>
-  </si>
-  <si>
     <t>Lengua Catalana y literatura</t>
   </si>
   <si>
@@ -136,9 +130,6 @@
   </si>
   <si>
     <t>Silvia S.</t>
-  </si>
-  <si>
-    <t>Total</t>
   </si>
   <si>
     <t>Andreu F.</t>
@@ -316,18 +307,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -355,7 +338,7 @@
       <name val="Calibri (Body)"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -377,12 +360,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -554,7 +531,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -562,10 +539,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -580,32 +557,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -617,7 +585,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -629,22 +597,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -653,30 +621,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -686,13 +657,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -713,7 +678,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1014,35 +979,35 @@
   </sheetPr>
   <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="33" customWidth="1"/>
+    <col min="1" max="1" width="9.125" style="30" customWidth="1"/>
     <col min="2" max="2" width="52.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="34" t="s">
-        <v>62</v>
+    <row r="1" spans="1:4">
+      <c r="A1" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="31" t="s">
+        <v>59</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>26</v>
@@ -1050,14 +1015,14 @@
       <c r="C2" s="5">
         <v>3</v>
       </c>
-      <c r="D2" s="43">
+      <c r="D2" s="41">
         <f>SUM(C2:C12)</f>
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="34" t="s">
-        <v>62</v>
+    <row r="3" spans="1:4" ht="17.100000000000001" customHeight="1">
+      <c r="A3" s="31" t="s">
+        <v>59</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>2</v>
@@ -1065,11 +1030,11 @@
       <c r="C3" s="5">
         <v>3</v>
       </c>
-      <c r="D3" s="43"/>
-    </row>
-    <row r="4" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="34" t="s">
-        <v>62</v>
+      <c r="D3" s="41"/>
+    </row>
+    <row r="4" spans="1:4" ht="17.100000000000001" customHeight="1">
+      <c r="A4" s="31" t="s">
+        <v>59</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>3</v>
@@ -1077,11 +1042,11 @@
       <c r="C4" s="5">
         <v>2</v>
       </c>
-      <c r="D4" s="43"/>
-    </row>
-    <row r="5" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="34" t="s">
-        <v>62</v>
+      <c r="D4" s="41"/>
+    </row>
+    <row r="5" spans="1:4" ht="17.100000000000001" customHeight="1">
+      <c r="A5" s="31" t="s">
+        <v>59</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>9</v>
@@ -1089,11 +1054,11 @@
       <c r="C5" s="5">
         <v>2</v>
       </c>
-      <c r="D5" s="43"/>
-    </row>
-    <row r="6" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="34" t="s">
-        <v>62</v>
+      <c r="D5" s="41"/>
+    </row>
+    <row r="6" spans="1:4" ht="17.100000000000001" customHeight="1">
+      <c r="A6" s="31" t="s">
+        <v>59</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>7</v>
@@ -1101,11 +1066,11 @@
       <c r="C6" s="5">
         <v>2</v>
       </c>
-      <c r="D6" s="43"/>
-    </row>
-    <row r="7" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="34" t="s">
-        <v>62</v>
+      <c r="D6" s="41"/>
+    </row>
+    <row r="7" spans="1:4" ht="17.100000000000001" customHeight="1">
+      <c r="A7" s="31" t="s">
+        <v>59</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>0</v>
@@ -1113,11 +1078,11 @@
       <c r="C7" s="5">
         <v>3</v>
       </c>
-      <c r="D7" s="43"/>
-    </row>
-    <row r="8" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="34" t="s">
-        <v>62</v>
+      <c r="D7" s="41"/>
+    </row>
+    <row r="8" spans="1:4" ht="17.100000000000001" customHeight="1">
+      <c r="A8" s="31" t="s">
+        <v>59</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>4</v>
@@ -1125,23 +1090,23 @@
       <c r="C8" s="5">
         <v>4</v>
       </c>
-      <c r="D8" s="43"/>
-    </row>
-    <row r="9" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="34" t="s">
-        <v>62</v>
+      <c r="D8" s="41"/>
+    </row>
+    <row r="9" spans="1:4" ht="17.100000000000001" customHeight="1">
+      <c r="A9" s="31" t="s">
+        <v>59</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C9" s="5">
         <v>4</v>
       </c>
-      <c r="D9" s="43"/>
-    </row>
-    <row r="10" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="34" t="s">
-        <v>62</v>
+      <c r="D9" s="41"/>
+    </row>
+    <row r="10" spans="1:4" ht="17.100000000000001" customHeight="1">
+      <c r="A10" s="31" t="s">
+        <v>59</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>5</v>
@@ -1149,11 +1114,11 @@
       <c r="C10" s="5">
         <v>4</v>
       </c>
-      <c r="D10" s="43"/>
-    </row>
-    <row r="11" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="34" t="s">
-        <v>62</v>
+      <c r="D10" s="41"/>
+    </row>
+    <row r="11" spans="1:4" ht="17.100000000000001" customHeight="1">
+      <c r="A11" s="31" t="s">
+        <v>59</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>6</v>
@@ -1161,11 +1126,11 @@
       <c r="C11" s="5">
         <v>2</v>
       </c>
-      <c r="D11" s="43"/>
-    </row>
-    <row r="12" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
-        <v>62</v>
+      <c r="D11" s="41"/>
+    </row>
+    <row r="12" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A12" s="31" t="s">
+        <v>59</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>1</v>
@@ -1173,11 +1138,11 @@
       <c r="C12" s="8">
         <v>1</v>
       </c>
-      <c r="D12" s="44"/>
-    </row>
-    <row r="13" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35" t="s">
-        <v>63</v>
+      <c r="D12" s="42"/>
+    </row>
+    <row r="13" spans="1:4" ht="18" customHeight="1" thickBot="1">
+      <c r="A13" s="32" t="s">
+        <v>60</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>26</v>
@@ -1185,14 +1150,14 @@
       <c r="C13" s="7">
         <v>3</v>
       </c>
-      <c r="D13" s="42">
+      <c r="D13" s="40">
         <f>SUM(C13:C23)</f>
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35" t="s">
-        <v>63</v>
+    <row r="14" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A14" s="32" t="s">
+        <v>60</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>2</v>
@@ -1200,11 +1165,11 @@
       <c r="C14" s="5">
         <v>3</v>
       </c>
-      <c r="D14" s="43"/>
-    </row>
-    <row r="15" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35" t="s">
-        <v>63</v>
+      <c r="D14" s="41"/>
+    </row>
+    <row r="15" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A15" s="32" t="s">
+        <v>60</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>3</v>
@@ -1212,11 +1177,11 @@
       <c r="C15" s="5">
         <v>2</v>
       </c>
-      <c r="D15" s="43"/>
-    </row>
-    <row r="16" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35" t="s">
-        <v>63</v>
+      <c r="D15" s="41"/>
+    </row>
+    <row r="16" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A16" s="32" t="s">
+        <v>60</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>8</v>
@@ -1224,11 +1189,11 @@
       <c r="C16" s="5">
         <v>2</v>
       </c>
-      <c r="D16" s="43"/>
-    </row>
-    <row r="17" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="35" t="s">
-        <v>63</v>
+      <c r="D16" s="41"/>
+    </row>
+    <row r="17" spans="1:4" ht="16.5" thickBot="1">
+      <c r="A17" s="32" t="s">
+        <v>60</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>7</v>
@@ -1236,11 +1201,11 @@
       <c r="C17" s="5">
         <v>2</v>
       </c>
-      <c r="D17" s="43"/>
-    </row>
-    <row r="18" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="35" t="s">
-        <v>63</v>
+      <c r="D17" s="41"/>
+    </row>
+    <row r="18" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A18" s="32" t="s">
+        <v>60</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>0</v>
@@ -1248,11 +1213,11 @@
       <c r="C18" s="5">
         <v>3</v>
       </c>
-      <c r="D18" s="43"/>
-    </row>
-    <row r="19" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="35" t="s">
-        <v>63</v>
+      <c r="D18" s="41"/>
+    </row>
+    <row r="19" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A19" s="32" t="s">
+        <v>60</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>4</v>
@@ -1260,23 +1225,23 @@
       <c r="C19" s="5">
         <v>4</v>
       </c>
-      <c r="D19" s="43"/>
-    </row>
-    <row r="20" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="35" t="s">
-        <v>63</v>
+      <c r="D19" s="41"/>
+    </row>
+    <row r="20" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A20" s="32" t="s">
+        <v>60</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C20" s="5">
         <v>4</v>
       </c>
-      <c r="D20" s="43"/>
-    </row>
-    <row r="21" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="35" t="s">
-        <v>63</v>
+      <c r="D20" s="41"/>
+    </row>
+    <row r="21" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A21" s="32" t="s">
+        <v>60</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>5</v>
@@ -1284,11 +1249,11 @@
       <c r="C21" s="5">
         <v>4</v>
       </c>
-      <c r="D21" s="43"/>
-    </row>
-    <row r="22" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="35" t="s">
-        <v>63</v>
+      <c r="D21" s="41"/>
+    </row>
+    <row r="22" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A22" s="32" t="s">
+        <v>60</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>10</v>
@@ -1296,11 +1261,11 @@
       <c r="C22" s="5">
         <v>2</v>
       </c>
-      <c r="D22" s="43"/>
-    </row>
-    <row r="23" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="35" t="s">
-        <v>63</v>
+      <c r="D22" s="41"/>
+    </row>
+    <row r="23" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A23" s="32" t="s">
+        <v>60</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>1</v>
@@ -1308,11 +1273,11 @@
       <c r="C23" s="8">
         <v>1</v>
       </c>
-      <c r="D23" s="44"/>
-    </row>
-    <row r="24" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="36" t="s">
-        <v>64</v>
+      <c r="D23" s="42"/>
+    </row>
+    <row r="24" spans="1:4" ht="18" customHeight="1" thickBot="1">
+      <c r="A24" s="33" t="s">
+        <v>61</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>26</v>
@@ -1320,14 +1285,14 @@
       <c r="C24" s="7">
         <v>2</v>
       </c>
-      <c r="D24" s="42">
+      <c r="D24" s="40">
         <f>SUM(C24:C35)</f>
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="36" t="s">
-        <v>64</v>
+    <row r="25" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A25" s="33" t="s">
+        <v>61</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>2</v>
@@ -1335,11 +1300,11 @@
       <c r="C25" s="5">
         <v>2</v>
       </c>
-      <c r="D25" s="43"/>
-    </row>
-    <row r="26" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="36" t="s">
-        <v>64</v>
+      <c r="D25" s="41"/>
+    </row>
+    <row r="26" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A26" s="33" t="s">
+        <v>61</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>3</v>
@@ -1347,11 +1312,11 @@
       <c r="C26" s="5">
         <v>2</v>
       </c>
-      <c r="D26" s="43"/>
-    </row>
-    <row r="27" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="36" t="s">
-        <v>64</v>
+      <c r="D26" s="41"/>
+    </row>
+    <row r="27" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A27" s="33" t="s">
+        <v>61</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>9</v>
@@ -1359,11 +1324,11 @@
       <c r="C27" s="5">
         <v>2</v>
       </c>
-      <c r="D27" s="43"/>
-    </row>
-    <row r="28" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="36" t="s">
-        <v>64</v>
+      <c r="D27" s="41"/>
+    </row>
+    <row r="28" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A28" s="33" t="s">
+        <v>61</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>10</v>
@@ -1371,11 +1336,11 @@
       <c r="C28" s="5">
         <v>3</v>
       </c>
-      <c r="D28" s="43"/>
-    </row>
-    <row r="29" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="36" t="s">
-        <v>64</v>
+      <c r="D28" s="41"/>
+    </row>
+    <row r="29" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A29" s="33" t="s">
+        <v>61</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>0</v>
@@ -1383,11 +1348,11 @@
       <c r="C29" s="5">
         <v>3</v>
       </c>
-      <c r="D29" s="43"/>
-    </row>
-    <row r="30" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="36" t="s">
-        <v>64</v>
+      <c r="D29" s="41"/>
+    </row>
+    <row r="30" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A30" s="33" t="s">
+        <v>61</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>4</v>
@@ -1395,23 +1360,23 @@
       <c r="C30" s="5">
         <v>4</v>
       </c>
-      <c r="D30" s="43"/>
-    </row>
-    <row r="31" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="36" t="s">
-        <v>64</v>
+      <c r="D30" s="41"/>
+    </row>
+    <row r="31" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A31" s="33" t="s">
+        <v>61</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C31" s="5">
         <v>4</v>
       </c>
-      <c r="D31" s="43"/>
-    </row>
-    <row r="32" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="36" t="s">
-        <v>64</v>
+      <c r="D31" s="41"/>
+    </row>
+    <row r="32" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A32" s="33" t="s">
+        <v>61</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>5</v>
@@ -1419,11 +1384,11 @@
       <c r="C32" s="5">
         <v>4</v>
       </c>
-      <c r="D32" s="43"/>
-    </row>
-    <row r="33" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="36" t="s">
-        <v>64</v>
+      <c r="D32" s="41"/>
+    </row>
+    <row r="33" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A33" s="33" t="s">
+        <v>61</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>6</v>
@@ -1431,11 +1396,11 @@
       <c r="C33" s="5">
         <v>2</v>
       </c>
-      <c r="D33" s="43"/>
-    </row>
-    <row r="34" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="36" t="s">
-        <v>64</v>
+      <c r="D33" s="41"/>
+    </row>
+    <row r="34" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A34" s="33" t="s">
+        <v>61</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>1</v>
@@ -1443,11 +1408,11 @@
       <c r="C34" s="5">
         <v>1</v>
       </c>
-      <c r="D34" s="43"/>
-    </row>
-    <row r="35" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="36" t="s">
-        <v>64</v>
+      <c r="D34" s="41"/>
+    </row>
+    <row r="35" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A35" s="33" t="s">
+        <v>61</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>11</v>
@@ -1455,11 +1420,11 @@
       <c r="C35" s="8">
         <v>1</v>
       </c>
-      <c r="D35" s="44"/>
-    </row>
-    <row r="36" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="37" t="s">
-        <v>65</v>
+      <c r="D35" s="42"/>
+    </row>
+    <row r="36" spans="1:4" ht="18" customHeight="1" thickBot="1">
+      <c r="A36" s="34" t="s">
+        <v>62</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>1</v>
@@ -1467,14 +1432,14 @@
       <c r="C36" s="7">
         <v>1</v>
       </c>
-      <c r="D36" s="42">
+      <c r="D36" s="40">
         <f>SUM(C36:C46)</f>
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="37" t="s">
-        <v>65</v>
+    <row r="37" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A37" s="34" t="s">
+        <v>62</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>2</v>
@@ -1482,11 +1447,11 @@
       <c r="C37" s="5">
         <v>3</v>
       </c>
-      <c r="D37" s="43"/>
-    </row>
-    <row r="38" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="37" t="s">
-        <v>65</v>
+      <c r="D37" s="41"/>
+    </row>
+    <row r="38" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A38" s="34" t="s">
+        <v>62</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>13</v>
@@ -1494,11 +1459,11 @@
       <c r="C38" s="5">
         <v>2</v>
       </c>
-      <c r="D38" s="43"/>
-    </row>
-    <row r="39" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="37" t="s">
-        <v>65</v>
+      <c r="D38" s="41"/>
+    </row>
+    <row r="39" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A39" s="34" t="s">
+        <v>62</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>3</v>
@@ -1506,11 +1471,11 @@
       <c r="C39" s="5">
         <v>2</v>
       </c>
-      <c r="D39" s="43"/>
-    </row>
-    <row r="40" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="37" t="s">
-        <v>65</v>
+      <c r="D39" s="41"/>
+    </row>
+    <row r="40" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A40" s="34" t="s">
+        <v>62</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>10</v>
@@ -1518,11 +1483,11 @@
       <c r="C40" s="5">
         <v>3</v>
       </c>
-      <c r="D40" s="43"/>
-    </row>
-    <row r="41" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="37" t="s">
-        <v>65</v>
+      <c r="D40" s="41"/>
+    </row>
+    <row r="41" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A41" s="34" t="s">
+        <v>62</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>0</v>
@@ -1530,11 +1495,11 @@
       <c r="C41" s="5">
         <v>3</v>
       </c>
-      <c r="D41" s="43"/>
-    </row>
-    <row r="42" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="37" t="s">
-        <v>65</v>
+      <c r="D41" s="41"/>
+    </row>
+    <row r="42" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A42" s="34" t="s">
+        <v>62</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>4</v>
@@ -1542,23 +1507,23 @@
       <c r="C42" s="5">
         <v>4</v>
       </c>
-      <c r="D42" s="43"/>
-    </row>
-    <row r="43" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="37" t="s">
-        <v>65</v>
+      <c r="D42" s="41"/>
+    </row>
+    <row r="43" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A43" s="34" t="s">
+        <v>62</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C43" s="5">
         <v>4</v>
       </c>
-      <c r="D43" s="43"/>
-    </row>
-    <row r="44" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="37" t="s">
-        <v>65</v>
+      <c r="D43" s="41"/>
+    </row>
+    <row r="44" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A44" s="34" t="s">
+        <v>62</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>14</v>
@@ -1566,11 +1531,11 @@
       <c r="C44" s="5">
         <v>2</v>
       </c>
-      <c r="D44" s="43"/>
-    </row>
-    <row r="45" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="37" t="s">
-        <v>65</v>
+      <c r="D44" s="41"/>
+    </row>
+    <row r="45" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A45" s="34" t="s">
+        <v>62</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>15</v>
@@ -1578,11 +1543,11 @@
       <c r="C45" s="5">
         <v>2</v>
       </c>
-      <c r="D45" s="43"/>
-    </row>
-    <row r="46" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="37" t="s">
-        <v>65</v>
+      <c r="D45" s="41"/>
+    </row>
+    <row r="46" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A46" s="34" t="s">
+        <v>62</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>12</v>
@@ -1590,11 +1555,11 @@
       <c r="C46" s="8">
         <v>4</v>
       </c>
-      <c r="D46" s="44"/>
-    </row>
-    <row r="47" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="38" t="s">
-        <v>66</v>
+      <c r="D46" s="42"/>
+    </row>
+    <row r="47" spans="1:4" ht="18" customHeight="1" thickBot="1">
+      <c r="A47" s="35" t="s">
+        <v>63</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>16</v>
@@ -1602,14 +1567,14 @@
       <c r="C47" s="7">
         <v>4</v>
       </c>
-      <c r="D47" s="42">
+      <c r="D47" s="40">
         <f>SUM(C47:C56)</f>
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="38" t="s">
-        <v>66</v>
+    <row r="48" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A48" s="35" t="s">
+        <v>63</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>17</v>
@@ -1617,11 +1582,11 @@
       <c r="C48" s="5">
         <v>3</v>
       </c>
-      <c r="D48" s="43"/>
-    </row>
-    <row r="49" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="38" t="s">
-        <v>66</v>
+      <c r="D48" s="41"/>
+    </row>
+    <row r="49" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A49" s="35" t="s">
+        <v>63</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>18</v>
@@ -1629,11 +1594,11 @@
       <c r="C49" s="5">
         <v>2</v>
       </c>
-      <c r="D49" s="43"/>
-    </row>
-    <row r="50" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="38" t="s">
-        <v>66</v>
+      <c r="D49" s="41"/>
+    </row>
+    <row r="50" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A50" s="35" t="s">
+        <v>63</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>3</v>
@@ -1641,11 +1606,11 @@
       <c r="C50" s="5">
         <v>2</v>
       </c>
-      <c r="D50" s="43"/>
-    </row>
-    <row r="51" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="38" t="s">
-        <v>66</v>
+      <c r="D50" s="41"/>
+    </row>
+    <row r="51" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A51" s="35" t="s">
+        <v>63</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>0</v>
@@ -1653,11 +1618,11 @@
       <c r="C51" s="5">
         <v>3</v>
       </c>
-      <c r="D51" s="43"/>
-    </row>
-    <row r="52" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="38" t="s">
-        <v>66</v>
+      <c r="D51" s="41"/>
+    </row>
+    <row r="52" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A52" s="35" t="s">
+        <v>63</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>19</v>
@@ -1665,11 +1630,11 @@
       <c r="C52" s="5">
         <v>2</v>
       </c>
-      <c r="D52" s="43"/>
-    </row>
-    <row r="53" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="38" t="s">
-        <v>66</v>
+      <c r="D52" s="41"/>
+    </row>
+    <row r="53" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A53" s="35" t="s">
+        <v>63</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>4</v>
@@ -1677,23 +1642,23 @@
       <c r="C53" s="5">
         <v>4</v>
       </c>
-      <c r="D53" s="43"/>
-    </row>
-    <row r="54" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="38" t="s">
-        <v>66</v>
+      <c r="D53" s="41"/>
+    </row>
+    <row r="54" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A54" s="35" t="s">
+        <v>63</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C54" s="5">
         <v>4</v>
       </c>
-      <c r="D54" s="43"/>
-    </row>
-    <row r="55" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="38" t="s">
-        <v>66</v>
+      <c r="D54" s="41"/>
+    </row>
+    <row r="55" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A55" s="35" t="s">
+        <v>63</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>20</v>
@@ -1701,11 +1666,11 @@
       <c r="C55" s="5">
         <v>3</v>
       </c>
-      <c r="D55" s="43"/>
-    </row>
-    <row r="56" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="38" t="s">
-        <v>66</v>
+      <c r="D55" s="41"/>
+    </row>
+    <row r="56" spans="1:4" ht="16.5" thickBot="1">
+      <c r="A56" s="35" t="s">
+        <v>63</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>14</v>
@@ -1713,11 +1678,11 @@
       <c r="C56" s="8">
         <v>3</v>
       </c>
-      <c r="D56" s="44"/>
-    </row>
-    <row r="57" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="39" t="s">
-        <v>67</v>
+      <c r="D56" s="42"/>
+    </row>
+    <row r="57" spans="1:4" ht="18" customHeight="1" thickBot="1">
+      <c r="A57" s="36" t="s">
+        <v>64</v>
       </c>
       <c r="B57" s="7" t="s">
         <v>22</v>
@@ -1725,14 +1690,14 @@
       <c r="C57" s="7">
         <v>4</v>
       </c>
-      <c r="D57" s="43">
+      <c r="D57" s="41">
         <f>SUM(C57:C65)</f>
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="39" t="s">
-        <v>67</v>
+    <row r="58" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A58" s="36" t="s">
+        <v>64</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>17</v>
@@ -1740,11 +1705,11 @@
       <c r="C58" s="5">
         <v>4</v>
       </c>
-      <c r="D58" s="43"/>
-    </row>
-    <row r="59" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="39" t="s">
-        <v>67</v>
+      <c r="D58" s="41"/>
+    </row>
+    <row r="59" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A59" s="36" t="s">
+        <v>64</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>23</v>
@@ -1752,11 +1717,11 @@
       <c r="C59" s="5">
         <v>3</v>
       </c>
-      <c r="D59" s="43"/>
-    </row>
-    <row r="60" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="39" t="s">
-        <v>67</v>
+      <c r="D59" s="41"/>
+    </row>
+    <row r="60" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A60" s="36" t="s">
+        <v>64</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>24</v>
@@ -1764,11 +1729,11 @@
       <c r="C60" s="5">
         <v>3</v>
       </c>
-      <c r="D60" s="43"/>
-    </row>
-    <row r="61" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="39" t="s">
-        <v>67</v>
+      <c r="D60" s="41"/>
+    </row>
+    <row r="61" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A61" s="36" t="s">
+        <v>64</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>0</v>
@@ -1776,11 +1741,11 @@
       <c r="C61" s="5">
         <v>4</v>
       </c>
-      <c r="D61" s="43"/>
-    </row>
-    <row r="62" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="39" t="s">
-        <v>67</v>
+      <c r="D61" s="41"/>
+    </row>
+    <row r="62" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A62" s="36" t="s">
+        <v>64</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>4</v>
@@ -1788,23 +1753,23 @@
       <c r="C62" s="5">
         <v>4</v>
       </c>
-      <c r="D62" s="43"/>
-    </row>
-    <row r="63" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="39" t="s">
-        <v>67</v>
+      <c r="D62" s="41"/>
+    </row>
+    <row r="63" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A63" s="36" t="s">
+        <v>64</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C63" s="5">
         <v>4</v>
       </c>
-      <c r="D63" s="43"/>
-    </row>
-    <row r="64" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="39" t="s">
-        <v>67</v>
+      <c r="D63" s="41"/>
+    </row>
+    <row r="64" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A64" s="36" t="s">
+        <v>64</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>25</v>
@@ -1812,11 +1777,11 @@
       <c r="C64" s="5">
         <v>2</v>
       </c>
-      <c r="D64" s="43"/>
-    </row>
-    <row r="65" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="39" t="s">
-        <v>67</v>
+      <c r="D64" s="41"/>
+    </row>
+    <row r="65" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A65" s="36" t="s">
+        <v>64</v>
       </c>
       <c r="B65" s="8" t="s">
         <v>21</v>
@@ -1824,9 +1789,9 @@
       <c r="C65" s="8">
         <v>2</v>
       </c>
-      <c r="D65" s="44"/>
-    </row>
-    <row r="66" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="D65" s="42"/>
+    </row>
+    <row r="66" spans="1:4" ht="18" customHeight="1"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="D36:D46"/>
@@ -1845,859 +1810,543 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1926007A-6418-CC4B-9DC0-43BC3D9D373B}">
   <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="46.5" style="1" customWidth="1"/>
-    <col min="2" max="4" width="17" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="17" style="1" customWidth="1"/>
+    <col min="3" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="9.625" customWidth="1"/>
+    <col min="6" max="6" width="10.875" customWidth="1"/>
+    <col min="7" max="7" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
-        <v>61</v>
+    <row r="1" spans="1:6">
+      <c r="A1" s="15" t="s">
+        <v>58</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>33</v>
-      </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5">
-        <f t="shared" ref="E2:E7" si="0">COUNTA(B2:D2)</f>
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="31.5">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="15.6" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5">
-        <f>COUNTA(C8:D8)</f>
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5">
-        <f t="shared" ref="E9:E29" si="1">COUNTA(B9:D9)</f>
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8">
       <c r="A17" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="5">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8">
       <c r="A18" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8">
       <c r="A19" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <v>75</v>
       </c>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8">
       <c r="A20" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E20" s="5">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8">
       <c r="A21" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8">
       <c r="A22" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8">
       <c r="A23" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E23" s="5">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8">
       <c r="A24" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>76</v>
       </c>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8">
       <c r="A25" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8">
       <c r="A26" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8">
       <c r="A27" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8">
       <c r="A28" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="40" t="s">
+    <row r="29" spans="1:8">
+      <c r="A29" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="41" t="s">
-        <v>60</v>
-      </c>
-      <c r="C29" s="41"/>
-      <c r="D29" s="41"/>
-      <c r="E29" s="41">
-        <f t="shared" si="1"/>
-        <v>1</v>
+      <c r="B29" s="38" t="s">
+        <v>57</v>
       </c>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="28"/>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="17"/>
+    <row r="30" spans="1:8">
+      <c r="A30" s="25"/>
+      <c r="B30" s="25"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="14"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
+    <row r="31" spans="1:8">
+      <c r="A31" s="12"/>
+      <c r="B31" s="12"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="14"/>
-      <c r="B32" s="28"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="15"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="14"/>
-      <c r="B33" s="16"/>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="46"/>
-      <c r="H33" s="15"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="26"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="46"/>
-      <c r="H34" s="15"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="26"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="15"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="26"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="25"/>
-      <c r="H36" s="15"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="26"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="15"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="26"/>
-      <c r="B38" s="20"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="25"/>
-      <c r="H38" s="15"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="26"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="25"/>
-      <c r="H39" s="15"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="26"/>
-      <c r="B40" s="20"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="25"/>
-      <c r="H40" s="15"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="26"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="25"/>
-      <c r="H41" s="15"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="26"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="25"/>
-      <c r="H42" s="15"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="26"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="25"/>
-      <c r="H43" s="15"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="26"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="25"/>
-      <c r="H44" s="15"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" s="26"/>
-      <c r="B45" s="20"/>
-      <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="25"/>
-      <c r="H45" s="15"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46" s="26"/>
-      <c r="B46" s="20"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="20"/>
-      <c r="G46" s="25"/>
-      <c r="H46" s="15"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A47" s="26"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="20"/>
-      <c r="G47" s="25"/>
-      <c r="H47" s="15"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" s="26"/>
-      <c r="B48" s="20"/>
-      <c r="C48" s="20"/>
-      <c r="D48" s="20"/>
-      <c r="E48" s="20"/>
-      <c r="F48" s="20"/>
-      <c r="G48" s="25"/>
-      <c r="H48" s="15"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="26"/>
-      <c r="B49" s="20"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="20"/>
-      <c r="G49" s="25"/>
-      <c r="H49" s="15"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="26"/>
-      <c r="B50" s="20"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="20"/>
-      <c r="G50" s="25"/>
-      <c r="H50" s="15"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="26"/>
-      <c r="B51" s="20"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
-      <c r="G51" s="25"/>
-      <c r="H51" s="15"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="26"/>
-      <c r="B52" s="20"/>
-      <c r="C52" s="20"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="20"/>
-      <c r="F52" s="20"/>
-      <c r="G52" s="25"/>
-      <c r="H52" s="15"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="26"/>
-      <c r="B53" s="20"/>
-      <c r="C53" s="20"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="20"/>
-      <c r="F53" s="20"/>
-      <c r="G53" s="25"/>
-      <c r="H53" s="15"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="26"/>
-      <c r="B54" s="20"/>
-      <c r="C54" s="20"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="20"/>
-      <c r="F54" s="20"/>
-      <c r="G54" s="25"/>
-      <c r="H54" s="15"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="26"/>
-      <c r="B55" s="20"/>
-      <c r="C55" s="20"/>
-      <c r="D55" s="20"/>
-      <c r="E55" s="20"/>
-      <c r="F55" s="20"/>
-      <c r="G55" s="25"/>
-      <c r="H55" s="15"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="26"/>
-      <c r="B56" s="20"/>
-      <c r="C56" s="20"/>
-      <c r="D56" s="20"/>
-      <c r="E56" s="20"/>
-      <c r="F56" s="20"/>
-      <c r="G56" s="25"/>
-      <c r="H56" s="15"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" s="26"/>
-      <c r="B57" s="20"/>
-      <c r="C57" s="20"/>
-      <c r="D57" s="20"/>
-      <c r="E57" s="20"/>
-      <c r="F57" s="20"/>
-      <c r="G57" s="25"/>
-      <c r="H57" s="15"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="26"/>
-      <c r="B58" s="20"/>
-      <c r="C58" s="20"/>
-      <c r="D58" s="20"/>
-      <c r="E58" s="20"/>
-      <c r="F58" s="20"/>
-      <c r="G58" s="25"/>
-      <c r="H58" s="15"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" s="26"/>
-      <c r="B59" s="20"/>
-      <c r="C59" s="14"/>
-      <c r="D59" s="20"/>
-      <c r="E59" s="20"/>
-      <c r="F59" s="20"/>
-      <c r="G59" s="25"/>
-      <c r="H59" s="15"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="26"/>
-      <c r="B60" s="20"/>
-      <c r="C60" s="20"/>
-      <c r="D60" s="20"/>
-      <c r="E60" s="20"/>
-      <c r="F60" s="20"/>
-      <c r="G60" s="25"/>
-      <c r="H60" s="15"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="26"/>
-      <c r="B61" s="20"/>
-      <c r="C61" s="20"/>
-      <c r="D61" s="20"/>
-      <c r="E61" s="20"/>
-      <c r="F61" s="20"/>
-      <c r="G61" s="25"/>
-      <c r="H61" s="15"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="26"/>
-      <c r="B62" s="20"/>
-      <c r="C62" s="20"/>
-      <c r="D62" s="20"/>
-      <c r="E62" s="20"/>
-      <c r="F62" s="20"/>
-      <c r="G62" s="25"/>
-      <c r="H62" s="15"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="26"/>
-      <c r="B63" s="20"/>
-      <c r="C63" s="20"/>
-      <c r="D63" s="20"/>
-      <c r="E63" s="20"/>
-      <c r="F63" s="20"/>
-      <c r="G63" s="25"/>
-      <c r="H63" s="15"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" s="27"/>
-      <c r="B64" s="20"/>
-      <c r="C64" s="20"/>
-      <c r="D64" s="20"/>
-      <c r="E64" s="20"/>
-      <c r="F64" s="20"/>
-      <c r="G64" s="25"/>
-      <c r="H64" s="15"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A65" s="14"/>
-      <c r="B65" s="14"/>
-      <c r="C65" s="14"/>
-      <c r="D65" s="14"/>
-      <c r="E65" s="14"/>
-      <c r="F65" s="21"/>
-      <c r="G65" s="25"/>
-      <c r="H65" s="15"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66" s="14"/>
-      <c r="B66" s="14"/>
-      <c r="C66" s="14"/>
-      <c r="D66" s="14"/>
-      <c r="E66" s="14"/>
-      <c r="F66" s="15"/>
-      <c r="G66" s="25"/>
-      <c r="H66" s="15"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F67" s="15"/>
-      <c r="G67" s="25"/>
-      <c r="H67" s="15"/>
+    <row r="32" spans="1:8">
+      <c r="A32" s="12"/>
+      <c r="B32" s="25"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="13"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="12"/>
+      <c r="B33" s="14"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="43"/>
+      <c r="H33" s="13"/>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="23"/>
+      <c r="B34" s="17"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="43"/>
+      <c r="H34" s="13"/>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="23"/>
+      <c r="B35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="13"/>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="23"/>
+      <c r="B36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="13"/>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="23"/>
+      <c r="B37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="13"/>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="23"/>
+      <c r="B38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="13"/>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="23"/>
+      <c r="B39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="13"/>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="23"/>
+      <c r="B40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="13"/>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="23"/>
+      <c r="B41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="22"/>
+      <c r="H41" s="13"/>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="23"/>
+      <c r="B42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="22"/>
+      <c r="H42" s="13"/>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="23"/>
+      <c r="B43" s="17"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="13"/>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="23"/>
+      <c r="B44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="13"/>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="23"/>
+      <c r="B45" s="17"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="22"/>
+      <c r="H45" s="13"/>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="23"/>
+      <c r="B46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="22"/>
+      <c r="H46" s="13"/>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="23"/>
+      <c r="B47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="22"/>
+      <c r="H47" s="13"/>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="23"/>
+      <c r="B48" s="17"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="22"/>
+      <c r="H48" s="13"/>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="23"/>
+      <c r="B49" s="17"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="22"/>
+      <c r="H49" s="13"/>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" s="23"/>
+      <c r="B50" s="17"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="22"/>
+      <c r="H50" s="13"/>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="23"/>
+      <c r="B51" s="17"/>
+      <c r="F51" s="17"/>
+      <c r="G51" s="22"/>
+      <c r="H51" s="13"/>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="23"/>
+      <c r="B52" s="17"/>
+      <c r="F52" s="17"/>
+      <c r="G52" s="22"/>
+      <c r="H52" s="13"/>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="23"/>
+      <c r="B53" s="17"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="22"/>
+      <c r="H53" s="13"/>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="23"/>
+      <c r="B54" s="17"/>
+      <c r="F54" s="17"/>
+      <c r="G54" s="22"/>
+      <c r="H54" s="13"/>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" s="23"/>
+      <c r="B55" s="17"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="22"/>
+      <c r="H55" s="13"/>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" s="23"/>
+      <c r="B56" s="17"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="22"/>
+      <c r="H56" s="13"/>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" s="23"/>
+      <c r="B57" s="17"/>
+      <c r="F57" s="17"/>
+      <c r="G57" s="22"/>
+      <c r="H57" s="13"/>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" s="23"/>
+      <c r="B58" s="17"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="22"/>
+      <c r="H58" s="13"/>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" s="23"/>
+      <c r="B59" s="17"/>
+      <c r="F59" s="17"/>
+      <c r="G59" s="22"/>
+      <c r="H59" s="13"/>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" s="23"/>
+      <c r="B60" s="17"/>
+      <c r="F60" s="17"/>
+      <c r="G60" s="22"/>
+      <c r="H60" s="13"/>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" s="23"/>
+      <c r="B61" s="17"/>
+      <c r="F61" s="17"/>
+      <c r="G61" s="22"/>
+      <c r="H61" s="13"/>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" s="23"/>
+      <c r="B62" s="17"/>
+      <c r="F62" s="17"/>
+      <c r="G62" s="22"/>
+      <c r="H62" s="13"/>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" s="23"/>
+      <c r="B63" s="17"/>
+      <c r="F63" s="17"/>
+      <c r="G63" s="22"/>
+      <c r="H63" s="13"/>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" s="24"/>
+      <c r="B64" s="17"/>
+      <c r="F64" s="17"/>
+      <c r="G64" s="22"/>
+      <c r="H64" s="13"/>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65" s="12"/>
+      <c r="B65" s="12"/>
+      <c r="F65" s="18"/>
+      <c r="G65" s="22"/>
+      <c r="H65" s="13"/>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" s="12"/>
+      <c r="B66" s="12"/>
+      <c r="F66" s="13"/>
+      <c r="G66" s="22"/>
+      <c r="H66" s="13"/>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="F67" s="13"/>
+      <c r="G67" s="22"/>
+      <c r="H67" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B30:D30"/>
+  <mergeCells count="1">
     <mergeCell ref="G33:G34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2707,506 +2356,505 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53966A10-ECE2-1349-837C-E1D3F35DE40D}">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView zoomScale="92" workbookViewId="0">
       <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="7" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="31" t="s">
-        <v>85</v>
+    <row r="1" spans="1:7">
+      <c r="A1" s="28" t="s">
+        <v>82</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G1" s="29" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="22" t="s">
-        <v>34</v>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="19" t="s">
+        <v>31</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F2" s="6"/>
-      <c r="G2" s="19">
+      <c r="G2" s="16">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
-        <v>58</v>
+    <row r="3" spans="1:7">
+      <c r="A3" s="19" t="s">
+        <v>55</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F3" s="6"/>
-      <c r="G3" s="19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
-        <v>36</v>
+      <c r="G3" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="19" t="s">
+        <v>33</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
-      <c r="G4" s="19">
+      <c r="G4" s="16">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="22" t="s">
-        <v>37</v>
+    <row r="5" spans="1:7">
+      <c r="A5" s="19" t="s">
+        <v>34</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
-      <c r="G5" s="19">
+      <c r="G5" s="16">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="22" t="s">
-        <v>75</v>
+    <row r="6" spans="1:7">
+      <c r="A6" s="19" t="s">
+        <v>72</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="19">
+      <c r="G6" s="16">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="22" t="s">
-        <v>76</v>
+    <row r="7" spans="1:7">
+      <c r="A7" s="19" t="s">
+        <v>73</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
-      <c r="G7" s="19">
+      <c r="G7" s="16">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="22" t="s">
-        <v>51</v>
+    <row r="8" spans="1:7">
+      <c r="A8" s="19" t="s">
+        <v>48</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
-      <c r="G8" s="19">
+      <c r="G8" s="16">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="22" t="s">
-        <v>77</v>
+    <row r="9" spans="1:7">
+      <c r="A9" s="19" t="s">
+        <v>74</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
-      <c r="G9" s="19">
+      <c r="G9" s="16">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="22" t="s">
-        <v>55</v>
+    <row r="10" spans="1:7" ht="31.5">
+      <c r="A10" s="19" t="s">
+        <v>52</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="19">
+      <c r="G10" s="16">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="22" t="s">
-        <v>52</v>
+    <row r="11" spans="1:7" ht="15.6" customHeight="1">
+      <c r="A11" s="19" t="s">
+        <v>49</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
-      <c r="G11" s="19">
+      <c r="G11" s="16">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="22" t="s">
-        <v>49</v>
+    <row r="12" spans="1:7">
+      <c r="A12" s="19" t="s">
+        <v>46</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F12" s="6"/>
-      <c r="G12" s="19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="22" t="s">
-        <v>54</v>
+      <c r="G12" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="19" t="s">
+        <v>51</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
-      <c r="G13" s="19">
+      <c r="G13" s="16">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="22" t="s">
-        <v>47</v>
+    <row r="14" spans="1:7">
+      <c r="A14" s="19" t="s">
+        <v>44</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
-      <c r="G14" s="19">
+      <c r="G14" s="16">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="22" t="s">
-        <v>35</v>
+    <row r="15" spans="1:7">
+      <c r="A15" s="19" t="s">
+        <v>32</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
-      <c r="G15" s="19">
+      <c r="G15" s="16">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="22" t="s">
-        <v>42</v>
+    <row r="16" spans="1:7">
+      <c r="A16" s="19" t="s">
+        <v>39</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G16" s="19">
+        <v>70</v>
+      </c>
+      <c r="G16" s="16">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="22" t="s">
-        <v>78</v>
+    <row r="17" spans="1:7">
+      <c r="A17" s="19" t="s">
+        <v>75</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G17" s="19">
+        <v>70</v>
+      </c>
+      <c r="G17" s="16">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="22" t="s">
-        <v>40</v>
+    <row r="18" spans="1:7">
+      <c r="A18" s="19" t="s">
+        <v>37</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
-      <c r="G18" s="19">
+      <c r="G18" s="16">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="22" t="s">
-        <v>79</v>
+    <row r="19" spans="1:7">
+      <c r="A19" s="19" t="s">
+        <v>76</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
-      <c r="G19" s="19">
+      <c r="G19" s="16">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="22" t="s">
-        <v>32</v>
+    <row r="20" spans="1:7">
+      <c r="A20" s="19" t="s">
+        <v>30</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
-      <c r="G20" s="19">
+      <c r="G20" s="16">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="22" t="s">
-        <v>45</v>
+    <row r="21" spans="1:7">
+      <c r="A21" s="19" t="s">
+        <v>42</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
-      <c r="G21" s="19">
+      <c r="G21" s="16">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="22" t="s">
-        <v>59</v>
+    <row r="22" spans="1:7">
+      <c r="A22" s="19" t="s">
+        <v>56</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G22" s="19">
+        <v>70</v>
+      </c>
+      <c r="G22" s="16">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="22" t="s">
-        <v>80</v>
+    <row r="23" spans="1:7">
+      <c r="A23" s="19" t="s">
+        <v>77</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
-      <c r="G23" s="19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="22" t="s">
-        <v>44</v>
+      <c r="G23" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
-      <c r="G24" s="19">
+      <c r="G24" s="16">
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="22" t="s">
-        <v>39</v>
+    <row r="25" spans="1:7">
+      <c r="A25" s="19" t="s">
+        <v>36</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
-      <c r="G25" s="19">
+      <c r="G25" s="16">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="22" t="s">
-        <v>50</v>
+    <row r="26" spans="1:7">
+      <c r="A26" s="19" t="s">
+        <v>47</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G26" s="19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="22" t="s">
-        <v>53</v>
+        <v>70</v>
+      </c>
+      <c r="G26" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="19" t="s">
+        <v>50</v>
       </c>
       <c r="B27" s="6"/>
       <c r="C27" s="1"/>
       <c r="D27" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
-      <c r="G27" s="19">
+      <c r="G27" s="16">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="22" t="s">
-        <v>48</v>
+    <row r="28" spans="1:7">
+      <c r="A28" s="19" t="s">
+        <v>45</v>
       </c>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
-      <c r="G28" s="19">
+      <c r="G28" s="16">
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="22" t="s">
-        <v>43</v>
+    <row r="29" spans="1:7">
+      <c r="A29" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
-      <c r="G29" s="19">
+      <c r="G29" s="16">
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="22" t="s">
-        <v>41</v>
+    <row r="30" spans="1:7">
+      <c r="A30" s="19" t="s">
+        <v>38</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F30" s="6"/>
-      <c r="G30" s="19">
+      <c r="G30" s="16">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="22" t="s">
-        <v>46</v>
+    <row r="31" spans="1:7">
+      <c r="A31" s="19" t="s">
+        <v>43</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
-      <c r="G31" s="19">
+      <c r="G31" s="16">
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="B32" s="23"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" ht="17" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:7">
+      <c r="A32" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="16">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3221,44 +2869,44 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="4" width="10.83203125" style="2"/>
-    <col min="5" max="5" width="39.1640625" style="2" customWidth="1"/>
+    <col min="1" max="4" width="10.875" style="2"/>
+    <col min="5" max="5" width="39.125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="C1" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="D1" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="E1" s="30" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E1" s="27" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="2">
         <v>5</v>
       </c>
       <c r="B2" s="2">
         <v>7</v>
       </c>
-      <c r="C2" s="47">
+      <c r="C2" s="39">
         <v>8</v>
       </c>
-      <c r="D2" s="47">
+      <c r="D2" s="39">
         <v>15</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ya funciona el algoritmo pero falta revisar
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\5-MUSI\Inteligencia Computacional\Timetable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreea/Desktop/20-21/1er Cuatrimestre/IC/Sebastián/Genetic_Timetable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA78AA5A-55C6-4718-A8BB-C5EFC6AC36CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D51F4661-0CE2-FC47-852D-B477A8CB10EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-12660" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{BC545386-80F0-1D4E-9D05-34C34264D497}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{BC545386-80F0-1D4E-9D05-34C34264D497}"/>
   </bookViews>
   <sheets>
     <sheet name="course_hours" sheetId="3" r:id="rId1"/>
@@ -307,7 +307,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -678,7 +678,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -979,19 +979,19 @@
   </sheetPr>
   <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.125" style="30" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" style="30" customWidth="1"/>
     <col min="2" max="2" width="52.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="29" t="s">
         <v>83</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
         <v>59</v>
       </c>
@@ -1020,7 +1020,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17.100000000000001" customHeight="1">
+    <row r="3" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
         <v>59</v>
       </c>
@@ -1032,7 +1032,7 @@
       </c>
       <c r="D3" s="41"/>
     </row>
-    <row r="4" spans="1:4" ht="17.100000000000001" customHeight="1">
+    <row r="4" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="31" t="s">
         <v>59</v>
       </c>
@@ -1044,7 +1044,7 @@
       </c>
       <c r="D4" s="41"/>
     </row>
-    <row r="5" spans="1:4" ht="17.100000000000001" customHeight="1">
+    <row r="5" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="31" t="s">
         <v>59</v>
       </c>
@@ -1056,7 +1056,7 @@
       </c>
       <c r="D5" s="41"/>
     </row>
-    <row r="6" spans="1:4" ht="17.100000000000001" customHeight="1">
+    <row r="6" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="31" t="s">
         <v>59</v>
       </c>
@@ -1068,7 +1068,7 @@
       </c>
       <c r="D6" s="41"/>
     </row>
-    <row r="7" spans="1:4" ht="17.100000000000001" customHeight="1">
+    <row r="7" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="31" t="s">
         <v>59</v>
       </c>
@@ -1080,7 +1080,7 @@
       </c>
       <c r="D7" s="41"/>
     </row>
-    <row r="8" spans="1:4" ht="17.100000000000001" customHeight="1">
+    <row r="8" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="31" t="s">
         <v>59</v>
       </c>
@@ -1092,7 +1092,7 @@
       </c>
       <c r="D8" s="41"/>
     </row>
-    <row r="9" spans="1:4" ht="17.100000000000001" customHeight="1">
+    <row r="9" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="31" t="s">
         <v>59</v>
       </c>
@@ -1104,7 +1104,7 @@
       </c>
       <c r="D9" s="41"/>
     </row>
-    <row r="10" spans="1:4" ht="17.100000000000001" customHeight="1">
+    <row r="10" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="31" t="s">
         <v>59</v>
       </c>
@@ -1116,7 +1116,7 @@
       </c>
       <c r="D10" s="41"/>
     </row>
-    <row r="11" spans="1:4" ht="17.100000000000001" customHeight="1">
+    <row r="11" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="31" t="s">
         <v>59</v>
       </c>
@@ -1128,7 +1128,7 @@
       </c>
       <c r="D11" s="41"/>
     </row>
-    <row r="12" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="12" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
         <v>59</v>
       </c>
@@ -1140,7 +1140,7 @@
       </c>
       <c r="D12" s="42"/>
     </row>
-    <row r="13" spans="1:4" ht="18" customHeight="1" thickBot="1">
+    <row r="13" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="32" t="s">
         <v>60</v>
       </c>
@@ -1155,7 +1155,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="14" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="32" t="s">
         <v>60</v>
       </c>
@@ -1167,7 +1167,7 @@
       </c>
       <c r="D14" s="41"/>
     </row>
-    <row r="15" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="15" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
         <v>60</v>
       </c>
@@ -1179,7 +1179,7 @@
       </c>
       <c r="D15" s="41"/>
     </row>
-    <row r="16" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="16" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="32" t="s">
         <v>60</v>
       </c>
@@ -1191,7 +1191,7 @@
       </c>
       <c r="D16" s="41"/>
     </row>
-    <row r="17" spans="1:4" ht="16.5" thickBot="1">
+    <row r="17" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="32" t="s">
         <v>60</v>
       </c>
@@ -1203,7 +1203,7 @@
       </c>
       <c r="D17" s="41"/>
     </row>
-    <row r="18" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="18" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="32" t="s">
         <v>60</v>
       </c>
@@ -1215,7 +1215,7 @@
       </c>
       <c r="D18" s="41"/>
     </row>
-    <row r="19" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="19" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="32" t="s">
         <v>60</v>
       </c>
@@ -1227,7 +1227,7 @@
       </c>
       <c r="D19" s="41"/>
     </row>
-    <row r="20" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="20" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="32" t="s">
         <v>60</v>
       </c>
@@ -1239,7 +1239,7 @@
       </c>
       <c r="D20" s="41"/>
     </row>
-    <row r="21" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="21" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="32" t="s">
         <v>60</v>
       </c>
@@ -1251,7 +1251,7 @@
       </c>
       <c r="D21" s="41"/>
     </row>
-    <row r="22" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="22" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="32" t="s">
         <v>60</v>
       </c>
@@ -1263,7 +1263,7 @@
       </c>
       <c r="D22" s="41"/>
     </row>
-    <row r="23" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="23" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="32" t="s">
         <v>60</v>
       </c>
@@ -1275,7 +1275,7 @@
       </c>
       <c r="D23" s="42"/>
     </row>
-    <row r="24" spans="1:4" ht="18" customHeight="1" thickBot="1">
+    <row r="24" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="33" t="s">
         <v>61</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="25" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="33" t="s">
         <v>61</v>
       </c>
@@ -1302,7 +1302,7 @@
       </c>
       <c r="D25" s="41"/>
     </row>
-    <row r="26" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="26" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="33" t="s">
         <v>61</v>
       </c>
@@ -1314,7 +1314,7 @@
       </c>
       <c r="D26" s="41"/>
     </row>
-    <row r="27" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="27" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="s">
         <v>61</v>
       </c>
@@ -1326,7 +1326,7 @@
       </c>
       <c r="D27" s="41"/>
     </row>
-    <row r="28" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="28" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="33" t="s">
         <v>61</v>
       </c>
@@ -1338,7 +1338,7 @@
       </c>
       <c r="D28" s="41"/>
     </row>
-    <row r="29" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="29" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="33" t="s">
         <v>61</v>
       </c>
@@ -1350,7 +1350,7 @@
       </c>
       <c r="D29" s="41"/>
     </row>
-    <row r="30" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="30" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="33" t="s">
         <v>61</v>
       </c>
@@ -1362,7 +1362,7 @@
       </c>
       <c r="D30" s="41"/>
     </row>
-    <row r="31" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="31" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="33" t="s">
         <v>61</v>
       </c>
@@ -1374,7 +1374,7 @@
       </c>
       <c r="D31" s="41"/>
     </row>
-    <row r="32" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="32" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="33" t="s">
         <v>61</v>
       </c>
@@ -1386,7 +1386,7 @@
       </c>
       <c r="D32" s="41"/>
     </row>
-    <row r="33" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="33" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="33" t="s">
         <v>61</v>
       </c>
@@ -1398,7 +1398,7 @@
       </c>
       <c r="D33" s="41"/>
     </row>
-    <row r="34" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="34" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="33" t="s">
         <v>61</v>
       </c>
@@ -1410,7 +1410,7 @@
       </c>
       <c r="D34" s="41"/>
     </row>
-    <row r="35" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="35" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="33" t="s">
         <v>61</v>
       </c>
@@ -1422,7 +1422,7 @@
       </c>
       <c r="D35" s="42"/>
     </row>
-    <row r="36" spans="1:4" ht="18" customHeight="1" thickBot="1">
+    <row r="36" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="34" t="s">
         <v>62</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="37" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="34" t="s">
         <v>62</v>
       </c>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="D37" s="41"/>
     </row>
-    <row r="38" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="38" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="34" t="s">
         <v>62</v>
       </c>
@@ -1461,7 +1461,7 @@
       </c>
       <c r="D38" s="41"/>
     </row>
-    <row r="39" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="39" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="34" t="s">
         <v>62</v>
       </c>
@@ -1473,7 +1473,7 @@
       </c>
       <c r="D39" s="41"/>
     </row>
-    <row r="40" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="40" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="34" t="s">
         <v>62</v>
       </c>
@@ -1485,7 +1485,7 @@
       </c>
       <c r="D40" s="41"/>
     </row>
-    <row r="41" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="41" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="34" t="s">
         <v>62</v>
       </c>
@@ -1497,7 +1497,7 @@
       </c>
       <c r="D41" s="41"/>
     </row>
-    <row r="42" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="42" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="34" t="s">
         <v>62</v>
       </c>
@@ -1509,7 +1509,7 @@
       </c>
       <c r="D42" s="41"/>
     </row>
-    <row r="43" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="43" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="34" t="s">
         <v>62</v>
       </c>
@@ -1521,7 +1521,7 @@
       </c>
       <c r="D43" s="41"/>
     </row>
-    <row r="44" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="44" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="34" t="s">
         <v>62</v>
       </c>
@@ -1533,7 +1533,7 @@
       </c>
       <c r="D44" s="41"/>
     </row>
-    <row r="45" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="45" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="34" t="s">
         <v>62</v>
       </c>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="D45" s="41"/>
     </row>
-    <row r="46" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="46" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="34" t="s">
         <v>62</v>
       </c>
@@ -1557,7 +1557,7 @@
       </c>
       <c r="D46" s="42"/>
     </row>
-    <row r="47" spans="1:4" ht="18" customHeight="1" thickBot="1">
+    <row r="47" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="35" t="s">
         <v>63</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="48" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="35" t="s">
         <v>63</v>
       </c>
@@ -1584,7 +1584,7 @@
       </c>
       <c r="D48" s="41"/>
     </row>
-    <row r="49" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="49" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="35" t="s">
         <v>63</v>
       </c>
@@ -1596,7 +1596,7 @@
       </c>
       <c r="D49" s="41"/>
     </row>
-    <row r="50" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="50" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="35" t="s">
         <v>63</v>
       </c>
@@ -1608,7 +1608,7 @@
       </c>
       <c r="D50" s="41"/>
     </row>
-    <row r="51" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="51" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="35" t="s">
         <v>63</v>
       </c>
@@ -1620,7 +1620,7 @@
       </c>
       <c r="D51" s="41"/>
     </row>
-    <row r="52" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="52" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="35" t="s">
         <v>63</v>
       </c>
@@ -1632,7 +1632,7 @@
       </c>
       <c r="D52" s="41"/>
     </row>
-    <row r="53" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="53" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="35" t="s">
         <v>63</v>
       </c>
@@ -1644,7 +1644,7 @@
       </c>
       <c r="D53" s="41"/>
     </row>
-    <row r="54" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="54" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="35" t="s">
         <v>63</v>
       </c>
@@ -1656,7 +1656,7 @@
       </c>
       <c r="D54" s="41"/>
     </row>
-    <row r="55" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="55" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="35" t="s">
         <v>63</v>
       </c>
@@ -1668,7 +1668,7 @@
       </c>
       <c r="D55" s="41"/>
     </row>
-    <row r="56" spans="1:4" ht="16.5" thickBot="1">
+    <row r="56" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="35" t="s">
         <v>63</v>
       </c>
@@ -1680,7 +1680,7 @@
       </c>
       <c r="D56" s="42"/>
     </row>
-    <row r="57" spans="1:4" ht="18" customHeight="1" thickBot="1">
+    <row r="57" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="36" t="s">
         <v>64</v>
       </c>
@@ -1695,7 +1695,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="58" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="36" t="s">
         <v>64</v>
       </c>
@@ -1707,7 +1707,7 @@
       </c>
       <c r="D58" s="41"/>
     </row>
-    <row r="59" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="59" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="36" t="s">
         <v>64</v>
       </c>
@@ -1719,7 +1719,7 @@
       </c>
       <c r="D59" s="41"/>
     </row>
-    <row r="60" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="60" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="36" t="s">
         <v>64</v>
       </c>
@@ -1731,7 +1731,7 @@
       </c>
       <c r="D60" s="41"/>
     </row>
-    <row r="61" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="61" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="36" t="s">
         <v>64</v>
       </c>
@@ -1743,7 +1743,7 @@
       </c>
       <c r="D61" s="41"/>
     </row>
-    <row r="62" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="62" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="36" t="s">
         <v>64</v>
       </c>
@@ -1755,7 +1755,7 @@
       </c>
       <c r="D62" s="41"/>
     </row>
-    <row r="63" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="63" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="36" t="s">
         <v>64</v>
       </c>
@@ -1767,7 +1767,7 @@
       </c>
       <c r="D63" s="41"/>
     </row>
-    <row r="64" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="64" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="36" t="s">
         <v>64</v>
       </c>
@@ -1779,7 +1779,7 @@
       </c>
       <c r="D64" s="41"/>
     </row>
-    <row r="65" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1">
+    <row r="65" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="36" t="s">
         <v>64</v>
       </c>
@@ -1791,7 +1791,7 @@
       </c>
       <c r="D65" s="42"/>
     </row>
-    <row r="66" spans="1:4" ht="18" customHeight="1"/>
+    <row r="66" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="D36:D46"/>
@@ -1810,21 +1810,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1926007A-6418-CC4B-9DC0-43BC3D9D373B}">
   <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="46.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="1" customWidth="1"/>
     <col min="3" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="9.625" customWidth="1"/>
-    <col min="6" max="6" width="10.875" customWidth="1"/>
-    <col min="7" max="7" width="10.875" style="2"/>
+    <col min="5" max="5" width="9.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>58</v>
       </c>
@@ -1833,7 +1833,7 @@
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>26</v>
       </c>
@@ -1842,7 +1842,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -1851,7 +1851,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1860,7 +1860,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -1869,7 +1869,7 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -1878,7 +1878,7 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="31.5">
+    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -1887,7 +1887,7 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" ht="15.6" customHeight="1">
+    <row r="8" spans="1:6" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -1896,7 +1896,7 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>25</v>
       </c>
@@ -1905,7 +1905,7 @@
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -1914,7 +1914,7 @@
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
@@ -1923,7 +1923,7 @@
       </c>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
@@ -1932,7 +1932,7 @@
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
@@ -1941,7 +1941,7 @@
       </c>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>23</v>
       </c>
@@ -1950,7 +1950,7 @@
       </c>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>24</v>
       </c>
@@ -1959,7 +1959,7 @@
       </c>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -1968,7 +1968,7 @@
       </c>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>0</v>
       </c>
@@ -1977,7 +1977,7 @@
       </c>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>4</v>
       </c>
@@ -1986,7 +1986,7 @@
       </c>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>28</v>
       </c>
@@ -1995,7 +1995,7 @@
       </c>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>5</v>
       </c>
@@ -2004,7 +2004,7 @@
       </c>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>16</v>
       </c>
@@ -2013,7 +2013,7 @@
       </c>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>22</v>
       </c>
@@ -2022,7 +2022,7 @@
       </c>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>12</v>
       </c>
@@ -2031,7 +2031,7 @@
       </c>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>6</v>
       </c>
@@ -2040,7 +2040,7 @@
       </c>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>1</v>
       </c>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>11</v>
       </c>
@@ -2058,7 +2058,7 @@
       </c>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>10</v>
       </c>
@@ -2067,7 +2067,7 @@
       </c>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>20</v>
       </c>
@@ -2076,7 +2076,7 @@
       </c>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="37" t="s">
         <v>17</v>
       </c>
@@ -2085,262 +2085,262 @@
       </c>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="25"/>
       <c r="B30" s="25"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="12"/>
       <c r="B31" s="12"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="12"/>
       <c r="B32" s="25"/>
       <c r="F32" s="13"/>
       <c r="G32" s="22"/>
       <c r="H32" s="13"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="12"/>
       <c r="B33" s="14"/>
       <c r="F33" s="12"/>
       <c r="G33" s="43"/>
       <c r="H33" s="13"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="23"/>
       <c r="B34" s="17"/>
       <c r="F34" s="14"/>
       <c r="G34" s="43"/>
       <c r="H34" s="13"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="23"/>
       <c r="B35" s="17"/>
       <c r="F35" s="17"/>
       <c r="G35" s="22"/>
       <c r="H35" s="13"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="23"/>
       <c r="B36" s="17"/>
       <c r="F36" s="17"/>
       <c r="G36" s="22"/>
       <c r="H36" s="13"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="23"/>
       <c r="B37" s="17"/>
       <c r="F37" s="17"/>
       <c r="G37" s="22"/>
       <c r="H37" s="13"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="23"/>
       <c r="B38" s="17"/>
       <c r="F38" s="17"/>
       <c r="G38" s="22"/>
       <c r="H38" s="13"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="23"/>
       <c r="B39" s="17"/>
       <c r="F39" s="17"/>
       <c r="G39" s="22"/>
       <c r="H39" s="13"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="23"/>
       <c r="B40" s="17"/>
       <c r="F40" s="17"/>
       <c r="G40" s="22"/>
       <c r="H40" s="13"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="23"/>
       <c r="B41" s="17"/>
       <c r="F41" s="17"/>
       <c r="G41" s="22"/>
       <c r="H41" s="13"/>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="23"/>
       <c r="B42" s="17"/>
       <c r="F42" s="17"/>
       <c r="G42" s="22"/>
       <c r="H42" s="13"/>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="23"/>
       <c r="B43" s="17"/>
       <c r="F43" s="17"/>
       <c r="G43" s="22"/>
       <c r="H43" s="13"/>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="23"/>
       <c r="B44" s="17"/>
       <c r="F44" s="17"/>
       <c r="G44" s="22"/>
       <c r="H44" s="13"/>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="23"/>
       <c r="B45" s="17"/>
       <c r="F45" s="17"/>
       <c r="G45" s="22"/>
       <c r="H45" s="13"/>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="23"/>
       <c r="B46" s="17"/>
       <c r="F46" s="17"/>
       <c r="G46" s="22"/>
       <c r="H46" s="13"/>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="23"/>
       <c r="B47" s="17"/>
       <c r="F47" s="17"/>
       <c r="G47" s="22"/>
       <c r="H47" s="13"/>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="23"/>
       <c r="B48" s="17"/>
       <c r="F48" s="17"/>
       <c r="G48" s="22"/>
       <c r="H48" s="13"/>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="23"/>
       <c r="B49" s="17"/>
       <c r="F49" s="17"/>
       <c r="G49" s="22"/>
       <c r="H49" s="13"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="23"/>
       <c r="B50" s="17"/>
       <c r="F50" s="17"/>
       <c r="G50" s="22"/>
       <c r="H50" s="13"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="23"/>
       <c r="B51" s="17"/>
       <c r="F51" s="17"/>
       <c r="G51" s="22"/>
       <c r="H51" s="13"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="23"/>
       <c r="B52" s="17"/>
       <c r="F52" s="17"/>
       <c r="G52" s="22"/>
       <c r="H52" s="13"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="23"/>
       <c r="B53" s="17"/>
       <c r="F53" s="17"/>
       <c r="G53" s="22"/>
       <c r="H53" s="13"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="23"/>
       <c r="B54" s="17"/>
       <c r="F54" s="17"/>
       <c r="G54" s="22"/>
       <c r="H54" s="13"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="23"/>
       <c r="B55" s="17"/>
       <c r="F55" s="17"/>
       <c r="G55" s="22"/>
       <c r="H55" s="13"/>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="23"/>
       <c r="B56" s="17"/>
       <c r="F56" s="17"/>
       <c r="G56" s="22"/>
       <c r="H56" s="13"/>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="23"/>
       <c r="B57" s="17"/>
       <c r="F57" s="17"/>
       <c r="G57" s="22"/>
       <c r="H57" s="13"/>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="23"/>
       <c r="B58" s="17"/>
       <c r="F58" s="17"/>
       <c r="G58" s="22"/>
       <c r="H58" s="13"/>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="23"/>
       <c r="B59" s="17"/>
       <c r="F59" s="17"/>
       <c r="G59" s="22"/>
       <c r="H59" s="13"/>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="23"/>
       <c r="B60" s="17"/>
       <c r="F60" s="17"/>
       <c r="G60" s="22"/>
       <c r="H60" s="13"/>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="23"/>
       <c r="B61" s="17"/>
       <c r="F61" s="17"/>
       <c r="G61" s="22"/>
       <c r="H61" s="13"/>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="23"/>
       <c r="B62" s="17"/>
       <c r="F62" s="17"/>
       <c r="G62" s="22"/>
       <c r="H62" s="13"/>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="23"/>
       <c r="B63" s="17"/>
       <c r="F63" s="17"/>
       <c r="G63" s="22"/>
       <c r="H63" s="13"/>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="24"/>
       <c r="B64" s="17"/>
       <c r="F64" s="17"/>
       <c r="G64" s="22"/>
       <c r="H64" s="13"/>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="12"/>
       <c r="B65" s="12"/>
       <c r="F65" s="18"/>
       <c r="G65" s="22"/>
       <c r="H65" s="13"/>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="12"/>
       <c r="B66" s="12"/>
       <c r="F66" s="13"/>
       <c r="G66" s="22"/>
       <c r="H66" s="13"/>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F67" s="13"/>
       <c r="G67" s="22"/>
       <c r="H67" s="13"/>
@@ -2362,12 +2362,12 @@
       <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="7" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="28" t="s">
         <v>82</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
         <v>31</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>55</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
         <v>33</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
         <v>34</v>
       </c>
@@ -2456,7 +2456,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
         <v>72</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
         <v>73</v>
       </c>
@@ -2490,7 +2490,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
         <v>48</v>
       </c>
@@ -2505,7 +2505,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
         <v>74</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="31.5">
+    <row r="10" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
         <v>52</v>
       </c>
@@ -2533,7 +2533,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.6" customHeight="1">
+    <row r="11" spans="1:7" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
         <v>49</v>
       </c>
@@ -2548,7 +2548,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
         <v>46</v>
       </c>
@@ -2563,7 +2563,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
         <v>51</v>
       </c>
@@ -2578,7 +2578,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
         <v>44</v>
       </c>
@@ -2591,7 +2591,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
         <v>32</v>
       </c>
@@ -2604,7 +2604,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
         <v>39</v>
       </c>
@@ -2619,7 +2619,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="19" t="s">
         <v>75</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="19" t="s">
         <v>37</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="19" t="s">
         <v>76</v>
       </c>
@@ -2662,7 +2662,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="19" t="s">
         <v>30</v>
       </c>
@@ -2675,7 +2675,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="19" t="s">
         <v>42</v>
       </c>
@@ -2688,7 +2688,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="19" t="s">
         <v>56</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="19" t="s">
         <v>77</v>
       </c>
@@ -2722,7 +2722,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="19" t="s">
         <v>41</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="19" t="s">
         <v>36</v>
       </c>
@@ -2752,7 +2752,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="19" t="s">
         <v>47</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
         <v>50</v>
       </c>
@@ -2782,7 +2782,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="19" t="s">
         <v>45</v>
       </c>
@@ -2795,7 +2795,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="19" t="s">
         <v>40</v>
       </c>
@@ -2810,7 +2810,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="19" t="s">
         <v>38</v>
       </c>
@@ -2827,7 +2827,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="19" t="s">
         <v>43</v>
       </c>
@@ -2842,7 +2842,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="19" t="s">
         <v>29</v>
       </c>
@@ -2869,13 +2869,13 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="10.875" style="2"/>
-    <col min="5" max="5" width="39.125" style="2" customWidth="1"/>
+    <col min="1" max="4" width="10.83203125" style="2"/>
+    <col min="5" max="5" width="39.1640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="27" t="s">
         <v>78</v>
       </c>
@@ -2892,7 +2892,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Modificada selección de padres con roulette wheel algorithm
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreea/Desktop/20-21/1er Cuatrimestre/IC/Sebastián/Genetic_Timetable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B988F6DE-03B6-AF45-BEC1-78733BE0C564}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7EC7A3-7CB1-8843-9D4C-025BDD1CC3C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16780" windowHeight="18000" activeTab="2" xr2:uid="{BC545386-80F0-1D4E-9D05-34C34264D497}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{BC545386-80F0-1D4E-9D05-34C34264D497}"/>
   </bookViews>
   <sheets>
     <sheet name="course_hours" sheetId="3" r:id="rId1"/>
     <sheet name="class_teachers" sheetId="2" r:id="rId2"/>
     <sheet name="teacher_hours" sheetId="4" r:id="rId3"/>
-    <sheet name="info" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId4"/>
+    <sheet name="info" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="265">
   <si>
     <t>Inglés</t>
   </si>
@@ -301,6 +302,537 @@
   </si>
   <si>
     <t>1ESO, 2ESO, 3ESO, 4ESO, 1BATX, 2BATX</t>
+  </si>
+  <si>
+    <t>LUNES 8 Educación física with Gloria F.</t>
+  </si>
+  <si>
+    <t>LUNES 9 Matemáticas with Eva M.</t>
+  </si>
+  <si>
+    <t>LUNES 10 Religión with Silvia S.</t>
+  </si>
+  <si>
+    <t>LUNES 12 Ciencias sociales, geografía e historia with Alexandre S.</t>
+  </si>
+  <si>
+    <t>LUNES 13 Ciencia de la naturaleza with Andreu F.</t>
+  </si>
+  <si>
+    <t>LUNES 14 Educación plástica y visual with Pere V.</t>
+  </si>
+  <si>
+    <t>MARTES 8 Inglés with Miquel B.</t>
+  </si>
+  <si>
+    <t>MARTES 9 Lengua Castellana y literatura with Carlos C.</t>
+  </si>
+  <si>
+    <t>MARTES 10 Educación física with Gloria F.</t>
+  </si>
+  <si>
+    <t>MARTES 11 Lengua Catalana y literatura with Esther C.</t>
+  </si>
+  <si>
+    <t>MARTES 12 Francés with Agathe N.</t>
+  </si>
+  <si>
+    <t>MARTES 13 Matemáticas with Eva M.</t>
+  </si>
+  <si>
+    <t>MARTES 14 Lengua Catalana y literatura with Esther C.</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES 9 Matemáticas with Eva M.</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES 11 Educación plástica y visual with Pere V.</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES 12 Música with María P.</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES 13 Ciencias sociales, geografía e historia with Alexandre S.</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES 14 Inglés with Miquel B.</t>
+  </si>
+  <si>
+    <t>JUEVES 8 Lengua Castellana y literatura with Carlos C.</t>
+  </si>
+  <si>
+    <t>JUEVES 9 Francés with Agathe N.</t>
+  </si>
+  <si>
+    <t>JUEVES 10 Ciencia de la naturaleza with Andreu F.</t>
+  </si>
+  <si>
+    <t>JUEVES 11 Ciencia de la naturaleza with Andreu F.</t>
+  </si>
+  <si>
+    <t>JUEVES 13 Lengua Castellana y literatura with Carlos C.</t>
+  </si>
+  <si>
+    <t>JUEVES 14 Música with María P.</t>
+  </si>
+  <si>
+    <t>VIERNES 8 Lengua Castellana y literatura with Carlos C.</t>
+  </si>
+  <si>
+    <t>VIERNES 9 Lengua Catalana y literatura with Esther C.</t>
+  </si>
+  <si>
+    <t>VIERNES 10 Matemáticas with Eva M.</t>
+  </si>
+  <si>
+    <t>VIERNES 11 Ciencias sociales, geografía e historia with Alexandre S.</t>
+  </si>
+  <si>
+    <t>VIERNES 12 Lengua Catalana y literatura with Esther C.</t>
+  </si>
+  <si>
+    <t>VIERNES 13 Inglés with Miquel B.</t>
+  </si>
+  <si>
+    <t>LUNES 8 Lengua Catalana y literatura with Esther C.</t>
+  </si>
+  <si>
+    <t>LUNES 9 Ciencias sociales, geografía e historia with Alexandre S.</t>
+  </si>
+  <si>
+    <t>LUNES 10 Matemáticas with Eva M.</t>
+  </si>
+  <si>
+    <t>LUNES 11 Lengua Catalana y literatura with Esther C.</t>
+  </si>
+  <si>
+    <t>LUNES 12 Ciencia de la naturaleza with Andreu F.</t>
+  </si>
+  <si>
+    <t>LUNES 13 Educación física with Gloria F.</t>
+  </si>
+  <si>
+    <t>LUNES 14 Lengua Castellana y literatura with Carlos C.</t>
+  </si>
+  <si>
+    <t>MARTES 8 Matemáticas with Eva M.</t>
+  </si>
+  <si>
+    <t>MARTES 9 Ciencia de la naturaleza with Andreu F.</t>
+  </si>
+  <si>
+    <t>MARTES 10 Ciencias sociales, geografía e historia with Alexandre S.</t>
+  </si>
+  <si>
+    <t>MARTES 11 Lengua Castellana y literatura with Carlos C.</t>
+  </si>
+  <si>
+    <t>MARTES 12 Ciencias sociales, geografía e historia with Alexandre S.</t>
+  </si>
+  <si>
+    <t>MARTES 13 Francés with Agathe N.</t>
+  </si>
+  <si>
+    <t>MARTES 14 Educación para la ciudadanía y los derechos humanos with Leonor A.</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES 8 Inglés with Miquel B.</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES 9 Francés with Agathe N.</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES 10 Educación física with Gloria F.</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES 11 Lengua Castellana y literatura with Carlos C.</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES 12 Lengua Catalana y literatura with Esther C.</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES 13 Matemáticas with Eva M.</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES 14 Educación para la ciudadanía y los derechos humanos with Leonor A.</t>
+  </si>
+  <si>
+    <t>JUEVES 8 Lengua Catalana y literatura with Esther C.</t>
+  </si>
+  <si>
+    <t>JUEVES 9 Lengua Castellana y literatura with Carlos C.</t>
+  </si>
+  <si>
+    <t>JUEVES 10 Inglés with Miquel B.</t>
+  </si>
+  <si>
+    <t>JUEVES 11 Religión with Silvia S.</t>
+  </si>
+  <si>
+    <t>JUEVES 12 Inglés with Miquel B.</t>
+  </si>
+  <si>
+    <t>JUEVES 13 Matemáticas with Eva M.</t>
+  </si>
+  <si>
+    <t>JUEVES 14 Tecnología with Xim H.</t>
+  </si>
+  <si>
+    <t>VIERNES 8 Ciencia de la naturaleza with Andreu F.</t>
+  </si>
+  <si>
+    <t>VIERNES 9 Tecnología with Xim H.</t>
+  </si>
+  <si>
+    <t>LUNES 8 Tecnología with Xim H.</t>
+  </si>
+  <si>
+    <t>LUNES 9 Tecnología with Xim H.</t>
+  </si>
+  <si>
+    <t>LUNES 10 Taller de ciéncias experimentales with Yolanda M.</t>
+  </si>
+  <si>
+    <t>LUNES 11 Lengua Castellana y literatura with Carlos C.</t>
+  </si>
+  <si>
+    <t>LUNES 12 Educación física with Gloria F.</t>
+  </si>
+  <si>
+    <t>LUNES 13 Matemáticas with Eva M.</t>
+  </si>
+  <si>
+    <t>LUNES 14 Inglés with Miquel B.</t>
+  </si>
+  <si>
+    <t>MARTES 9 Matemáticas with Eva M.</t>
+  </si>
+  <si>
+    <t>MARTES 10 Lengua Catalana y literatura with Esther C.</t>
+  </si>
+  <si>
+    <t>MARTES 11 Matemáticas with Eva M.</t>
+  </si>
+  <si>
+    <t>MARTES 12 Educación plástica y visual with Pere V.</t>
+  </si>
+  <si>
+    <t>MARTES 13 Lengua Catalana y literatura with Esther C.</t>
+  </si>
+  <si>
+    <t>MARTES 14 Lengua Castellana y literatura with Carlos C.</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES 8 Lengua Castellana y literatura with Carlos C.</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES 9 Educación física with Gloria F.</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES 10 Ciencia de la naturaleza with Andreu F.</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES 12 Lengua Castellana y literatura with Carlos C.</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES 13 Educación plástica y visual with Pere V.</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES 14 Ciencias sociales, geografía e historia with Alexandre S.</t>
+  </si>
+  <si>
+    <t>JUEVES 8 Ciencia de la naturaleza with Andreu F.</t>
+  </si>
+  <si>
+    <t>JUEVES 9 Lengua Catalana y literatura with Esther C.</t>
+  </si>
+  <si>
+    <t>JUEVES 11 Música with María P.</t>
+  </si>
+  <si>
+    <t>JUEVES 12 Tecnología with Xim H.</t>
+  </si>
+  <si>
+    <t>JUEVES 13 Inglés with Miquel B.</t>
+  </si>
+  <si>
+    <t>JUEVES 14 Ciencias sociales, geografía e historia with Alexandre S.</t>
+  </si>
+  <si>
+    <t>VIERNES 8 Inglés with Miquel B.</t>
+  </si>
+  <si>
+    <t>VIERNES 9 Religión with Silvia S.</t>
+  </si>
+  <si>
+    <t>VIERNES 10 Lengua Catalana y literatura with Esther C.</t>
+  </si>
+  <si>
+    <t>VIERNES 13 Matemáticas with Eva M.</t>
+  </si>
+  <si>
+    <t>VIERNES 14 Música with María P.</t>
+  </si>
+  <si>
+    <t>LUNES 8 Física y química with Ángel F.</t>
+  </si>
+  <si>
+    <t>LUNES 9 Educación eticocívica with Pedro P.</t>
+  </si>
+  <si>
+    <t>LUNES 11 Matemáticas B with Llorenç S.</t>
+  </si>
+  <si>
+    <t>LUNES 12 Lengua Castellana y literatura with Carlos C.</t>
+  </si>
+  <si>
+    <t>LUNES 13 Educación eticocívica with Pedro P.</t>
+  </si>
+  <si>
+    <t>LUNES 14 Lengua Catalana y literatura with Esther C.</t>
+  </si>
+  <si>
+    <t>MARTES 8 Matemáticas B with Llorenç S.</t>
+  </si>
+  <si>
+    <t>MARTES 9 Informática with Llorenç S.</t>
+  </si>
+  <si>
+    <t>MARTES 10 Matemáticas B with Llorenç S.</t>
+  </si>
+  <si>
+    <t>MARTES 11 Tecnología with Xim H.</t>
+  </si>
+  <si>
+    <t>MARTES 12 Inglés with Miquel B.</t>
+  </si>
+  <si>
+    <t>MARTES 13 Educación física with Gloria F.</t>
+  </si>
+  <si>
+    <t>MARTES 14 Informática with Llorenç S.</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES 9 Inglés with Miquel B.</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES 10 Tecnología with Xim H.</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES 11 Ciencias sociales, geografía e historia with Alexandre S.</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES 13 Lengua Castellana y literatura with Carlos C.</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES 14 Lengua Catalana y literatura with Esther C.</t>
+  </si>
+  <si>
+    <t>JUEVES 8 Tecnología with Xim H.</t>
+  </si>
+  <si>
+    <t>JUEVES 9 Educación física with Gloria F.</t>
+  </si>
+  <si>
+    <t>JUEVES 10 Lengua Catalana y literatura with Esther C.</t>
+  </si>
+  <si>
+    <t>JUEVES 11 Lengua Catalana y literatura with Esther C.</t>
+  </si>
+  <si>
+    <t>JUEVES 12 Física y química with Ángel F.</t>
+  </si>
+  <si>
+    <t>JUEVES 14 Matemáticas B with Llorenç S.</t>
+  </si>
+  <si>
+    <t>VIERNES 8 Ciencias sociales, geografía e historia with Alexandre S.</t>
+  </si>
+  <si>
+    <t>VIERNES 10 Lengua Castellana y literatura with Carlos C.</t>
+  </si>
+  <si>
+    <t>VIERNES 11 Inglés with Miquel B.</t>
+  </si>
+  <si>
+    <t>VIERNES 12 Ciencias sociales, geografía e historia with Alexandre S.</t>
+  </si>
+  <si>
+    <t>VIERNES 13 Religión with Silvia S.</t>
+  </si>
+  <si>
+    <t>VIERNES 14 Lengua Castellana y literatura with Carlos C.</t>
+  </si>
+  <si>
+    <t>LUNES 8 Tecnología de la información y la comunicación with Carmen R.</t>
+  </si>
+  <si>
+    <t>LUNES 9 Matemáticas 1 with Cristina O.</t>
+  </si>
+  <si>
+    <t>LUNES 10 Inglés with Miquel B.</t>
+  </si>
+  <si>
+    <t>LUNES 12 Matemáticas 1 with Cristina O.</t>
+  </si>
+  <si>
+    <t>LUNES 13 Lengua Catalana y literatura with Esther C.</t>
+  </si>
+  <si>
+    <t>LUNES 14 Educación física with Gloria F.</t>
+  </si>
+  <si>
+    <t>MARTES 8 Lengua Catalana y literatura with Esther C.</t>
+  </si>
+  <si>
+    <t>MARTES 9 Inglés with Miquel B.</t>
+  </si>
+  <si>
+    <t>MARTES 10 Lengua Castellana y literatura with Carlos C.</t>
+  </si>
+  <si>
+    <t>MARTES 12 Lengua Catalana y literatura with Esther C.</t>
+  </si>
+  <si>
+    <t>MARTES 14 Tecnología de la información y la comunicación with Carmen R.</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES 8 Educación física with Gloria F.</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES 10 Lengua Castellana y literatura with Carlos C.</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES 11 Física y química with Ángel F.</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES 12 Inglés with Miquel B.</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES 13 Ciéncias para el mundo contemporáneo with Cristina B.</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES 14 Tecnología industrial with Yolanda M.</t>
+  </si>
+  <si>
+    <t>JUEVES 8 Filosofia y ciutadania with Maria Teresa L.</t>
+  </si>
+  <si>
+    <t>JUEVES 9 Tecnología de la información y la comunicación with Carmen R.</t>
+  </si>
+  <si>
+    <t>JUEVES 10 Física y química with Ángel F.</t>
+  </si>
+  <si>
+    <t>JUEVES 11 Física y química with Ángel F.</t>
+  </si>
+  <si>
+    <t>JUEVES 12 Matemáticas 1 with Cristina O.</t>
+  </si>
+  <si>
+    <t>JUEVES 13 Filosofia y ciutadania with Maria Teresa L.</t>
+  </si>
+  <si>
+    <t>VIERNES 8 Matemáticas 1 with Cristina O.</t>
+  </si>
+  <si>
+    <t>VIERNES 9 Tecnología industrial with Yolanda M.</t>
+  </si>
+  <si>
+    <t>VIERNES 10 Tecnología industrial with Yolanda M.</t>
+  </si>
+  <si>
+    <t>VIERNES 14 Ciéncias para el mundo contemporáneo with Cristina B.</t>
+  </si>
+  <si>
+    <t>LUNES 8 Lengua Castellana y literatura with Carlos C.</t>
+  </si>
+  <si>
+    <t>LUNES 9 Tecnología industrial with Yolanda M.</t>
+  </si>
+  <si>
+    <t>LUNES 10 Lengua Castellana y literatura with Carlos C.</t>
+  </si>
+  <si>
+    <t>LUNES 11 Inglés with Miquel B.</t>
+  </si>
+  <si>
+    <t>LUNES 12 Historia de la filosofia with Carlos S.</t>
+  </si>
+  <si>
+    <t>LUNES 13 Inglés with Miquel B.</t>
+  </si>
+  <si>
+    <t>LUNES 14 Tecnología industrial with Yolanda M.</t>
+  </si>
+  <si>
+    <t>MARTES 8 Historia de España with Alexandre S.</t>
+  </si>
+  <si>
+    <t>MARTES 9 Historia de la filosofia with Carlos S.</t>
+  </si>
+  <si>
+    <t>MARTES 10 Inglés with Miquel B.</t>
+  </si>
+  <si>
+    <t>MARTES 11 Tecnología industrial with Yolanda M.</t>
+  </si>
+  <si>
+    <t>MARTES 12 Física with Ángel F.</t>
+  </si>
+  <si>
+    <t>MARTES 13 Inglés with Miquel B.</t>
+  </si>
+  <si>
+    <t>MARTES 14 Historia de España with Alexandre S.</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES 8 Física with Ángel F.</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES 9 Lengua Catalana y literatura with Esther C.</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES 11 Electrotécnia with Ruth B.</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES 12 Historia de España with Alexandre S.</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES 14 Matemáticas 2 with Eva M.</t>
+  </si>
+  <si>
+    <t>JUEVES 8 Historia de la filosofia with Carlos S.</t>
+  </si>
+  <si>
+    <t>JUEVES 9 Tecnología industrial with Yolanda M.</t>
+  </si>
+  <si>
+    <t>JUEVES 11 Lengua Castellana y literatura with Carlos C.</t>
+  </si>
+  <si>
+    <t>JUEVES 12 Lengua Castellana y literatura with Carlos C.</t>
+  </si>
+  <si>
+    <t>JUEVES 13 Lengua Catalana y literatura with Esther C.</t>
+  </si>
+  <si>
+    <t>JUEVES 14 Matemáticas 2 with Eva M.</t>
+  </si>
+  <si>
+    <t>VIERNES 8 Matemáticas 2 with Eva M.</t>
+  </si>
+  <si>
+    <t>VIERNES 9 Matemáticas 2 with Eva M.</t>
+  </si>
+  <si>
+    <t>VIERNES 10 Electrotécnia with Ruth B.</t>
+  </si>
+  <si>
+    <t>VIERNES 11 Lengua Catalana y literatura with Esther C.</t>
+  </si>
+  <si>
+    <t>VIERNES 13 Lengua Catalana y literatura with Esther C.</t>
   </si>
 </sst>
 </file>
@@ -338,7 +870,7 @@
       <name val="Calibri (Body)"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -402,6 +934,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -531,7 +1075,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -660,6 +1204,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2358,8 +2905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53966A10-ECE2-1349-837C-E1D3F35DE40D}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView zoomScale="92" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2834,6 +3381,809 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3942144A-E313-9B4E-BEA7-992818B28456}">
+  <dimension ref="A1:AD35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="54" zoomScaleNormal="54" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="41" customWidth="1"/>
+    <col min="8" max="8" width="36.5" customWidth="1"/>
+    <col min="13" max="13" width="16.1640625" customWidth="1"/>
+    <col min="16" max="16" width="40.6640625" customWidth="1"/>
+    <col min="17" max="17" width="24.1640625" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="0.1640625" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="15.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A1" s="46" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I1" t="s">
+        <v>148</v>
+      </c>
+      <c r="N1" s="46" t="s">
+        <v>178</v>
+      </c>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="T1" t="s">
+        <v>208</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="46" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" t="s">
+        <v>149</v>
+      </c>
+      <c r="N2" t="s">
+        <v>179</v>
+      </c>
+      <c r="T2" t="s">
+        <v>209</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" t="s">
+        <v>120</v>
+      </c>
+      <c r="I3" t="s">
+        <v>150</v>
+      </c>
+      <c r="T3" t="s">
+        <v>210</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>121</v>
+      </c>
+      <c r="I4" s="44" t="s">
+        <v>151</v>
+      </c>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="44"/>
+      <c r="N4" t="s">
+        <v>180</v>
+      </c>
+      <c r="T4" s="44" t="s">
+        <v>151</v>
+      </c>
+      <c r="U4" s="44"/>
+      <c r="V4" s="44"/>
+      <c r="W4" s="44"/>
+      <c r="X4" s="44"/>
+      <c r="Z4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A5" s="46" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="45" t="s">
+        <v>122</v>
+      </c>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="I5" s="46" t="s">
+        <v>152</v>
+      </c>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="46"/>
+      <c r="N5" s="45" t="s">
+        <v>181</v>
+      </c>
+      <c r="O5" s="45"/>
+      <c r="P5" s="45"/>
+      <c r="Q5" s="44"/>
+      <c r="R5" s="44"/>
+      <c r="S5" s="44"/>
+      <c r="T5" t="s">
+        <v>211</v>
+      </c>
+      <c r="Z5" s="45" t="s">
+        <v>239</v>
+      </c>
+      <c r="AA5" s="45"/>
+      <c r="AB5" s="45"/>
+      <c r="AC5" s="45"/>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="45"/>
+      <c r="D6" s="46" t="s">
+        <v>123</v>
+      </c>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" t="s">
+        <v>153</v>
+      </c>
+      <c r="N6" t="s">
+        <v>182</v>
+      </c>
+      <c r="T6" s="45" t="s">
+        <v>212</v>
+      </c>
+      <c r="U6" s="45"/>
+      <c r="V6" s="45"/>
+      <c r="W6" s="45"/>
+      <c r="X6" s="45"/>
+      <c r="Z6" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A7" s="46" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
+      <c r="D7" t="s">
+        <v>124</v>
+      </c>
+      <c r="I7" t="s">
+        <v>154</v>
+      </c>
+      <c r="N7" t="s">
+        <v>183</v>
+      </c>
+      <c r="P7" s="45"/>
+      <c r="Q7" s="45"/>
+      <c r="R7" s="45"/>
+      <c r="S7" s="45"/>
+      <c r="T7" s="46" t="s">
+        <v>213</v>
+      </c>
+      <c r="U7" s="46"/>
+      <c r="V7" s="46"/>
+      <c r="W7" s="46"/>
+      <c r="X7" s="46"/>
+      <c r="Y7" s="46"/>
+      <c r="Z7" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" s="46" t="s">
+        <v>125</v>
+      </c>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="N8" t="s">
+        <v>184</v>
+      </c>
+      <c r="T8" t="s">
+        <v>214</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" s="46" t="s">
+        <v>126</v>
+      </c>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46" t="s">
+        <v>155</v>
+      </c>
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="46"/>
+      <c r="M9" s="46"/>
+      <c r="N9" t="s">
+        <v>185</v>
+      </c>
+      <c r="T9" t="s">
+        <v>215</v>
+      </c>
+      <c r="Z9" s="46" t="s">
+        <v>243</v>
+      </c>
+      <c r="AA9" s="46"/>
+      <c r="AB9" s="46"/>
+      <c r="AC9" s="46"/>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" t="s">
+        <v>127</v>
+      </c>
+      <c r="I10" t="s">
+        <v>156</v>
+      </c>
+      <c r="N10" t="s">
+        <v>186</v>
+      </c>
+      <c r="T10" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" t="s">
+        <v>157</v>
+      </c>
+      <c r="N11" t="s">
+        <v>187</v>
+      </c>
+      <c r="T11" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="U11" s="44"/>
+      <c r="V11" s="44"/>
+      <c r="W11" s="44"/>
+      <c r="X11" s="44"/>
+      <c r="Y11" s="44"/>
+      <c r="Z11" s="46" t="s">
+        <v>245</v>
+      </c>
+      <c r="AA11" s="46"/>
+      <c r="AB11" s="46"/>
+      <c r="AC11" s="46"/>
+      <c r="AD11" s="46"/>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" t="s">
+        <v>129</v>
+      </c>
+      <c r="I12" t="s">
+        <v>158</v>
+      </c>
+      <c r="N12" t="s">
+        <v>188</v>
+      </c>
+      <c r="T12" t="s">
+        <v>217</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>99</v>
+      </c>
+      <c r="D13" t="s">
+        <v>130</v>
+      </c>
+      <c r="I13" s="44" t="s">
+        <v>159</v>
+      </c>
+      <c r="J13" s="44"/>
+      <c r="K13" s="44"/>
+      <c r="L13" s="44"/>
+      <c r="M13" s="44"/>
+      <c r="N13" t="s">
+        <v>189</v>
+      </c>
+      <c r="T13" s="44" t="s">
+        <v>159</v>
+      </c>
+      <c r="U13" s="44"/>
+      <c r="V13" s="44"/>
+      <c r="W13" s="44"/>
+      <c r="X13" s="44"/>
+      <c r="Y13" s="44"/>
+      <c r="Z13" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" s="46" t="s">
+        <v>131</v>
+      </c>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="46"/>
+      <c r="I14" t="s">
+        <v>160</v>
+      </c>
+      <c r="N14" t="s">
+        <v>190</v>
+      </c>
+      <c r="T14" t="s">
+        <v>218</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>132</v>
+      </c>
+      <c r="I15" t="s">
+        <v>161</v>
+      </c>
+      <c r="T15" s="46" t="s">
+        <v>219</v>
+      </c>
+      <c r="U15" s="46"/>
+      <c r="V15" s="46"/>
+      <c r="W15" s="46"/>
+      <c r="X15" s="46"/>
+      <c r="Y15" s="46"/>
+      <c r="Z15" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>101</v>
+      </c>
+      <c r="D16" t="s">
+        <v>133</v>
+      </c>
+      <c r="I16" s="46" t="s">
+        <v>162</v>
+      </c>
+      <c r="J16" s="46"/>
+      <c r="K16" s="46"/>
+      <c r="L16" s="46"/>
+      <c r="M16" s="46"/>
+      <c r="N16" t="s">
+        <v>191</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="D17" s="46" t="s">
+        <v>134</v>
+      </c>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" t="s">
+        <v>163</v>
+      </c>
+      <c r="N17" t="s">
+        <v>192</v>
+      </c>
+      <c r="T17" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" t="s">
+        <v>135</v>
+      </c>
+      <c r="N18" s="46" t="s">
+        <v>193</v>
+      </c>
+      <c r="O18" s="46"/>
+      <c r="P18" s="46"/>
+      <c r="T18" t="s">
+        <v>221</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>103</v>
+      </c>
+      <c r="D19" t="s">
+        <v>136</v>
+      </c>
+      <c r="I19" t="s">
+        <v>164</v>
+      </c>
+      <c r="T19" t="s">
+        <v>222</v>
+      </c>
+      <c r="Z19" s="46" t="s">
+        <v>252</v>
+      </c>
+      <c r="AA19" s="46"/>
+      <c r="AB19" s="46"/>
+      <c r="AC19" s="46"/>
+      <c r="AD19" s="46"/>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A20" s="46" t="s">
+        <v>104</v>
+      </c>
+      <c r="B20" s="46"/>
+      <c r="C20" s="46"/>
+      <c r="D20" t="s">
+        <v>137</v>
+      </c>
+      <c r="I20" t="s">
+        <v>165</v>
+      </c>
+      <c r="N20" t="s">
+        <v>194</v>
+      </c>
+      <c r="T20" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>105</v>
+      </c>
+      <c r="D21" s="46" t="s">
+        <v>138</v>
+      </c>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="46" t="s">
+        <v>166</v>
+      </c>
+      <c r="J21" s="46"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="46"/>
+      <c r="M21" s="46"/>
+      <c r="N21" t="s">
+        <v>195</v>
+      </c>
+      <c r="T21" s="46" t="s">
+        <v>224</v>
+      </c>
+      <c r="U21" s="46"/>
+      <c r="V21" s="46"/>
+      <c r="W21" s="46"/>
+      <c r="X21" s="46"/>
+      <c r="Y21" s="46"/>
+      <c r="Z21" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>106</v>
+      </c>
+      <c r="D22" t="s">
+        <v>139</v>
+      </c>
+      <c r="I22" s="46" t="s">
+        <v>167</v>
+      </c>
+      <c r="J22" s="46"/>
+      <c r="K22" s="46"/>
+      <c r="L22" s="46"/>
+      <c r="M22" s="46"/>
+      <c r="N22" t="s">
+        <v>196</v>
+      </c>
+      <c r="T22" t="s">
+        <v>225</v>
+      </c>
+      <c r="Z22" s="45" t="s">
+        <v>254</v>
+      </c>
+      <c r="AA22" s="45"/>
+      <c r="AB22" s="45"/>
+      <c r="AC22" s="45"/>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A23" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="B23" s="46"/>
+      <c r="C23" s="46"/>
+      <c r="D23" t="s">
+        <v>140</v>
+      </c>
+      <c r="I23" t="s">
+        <v>168</v>
+      </c>
+      <c r="N23" t="s">
+        <v>197</v>
+      </c>
+      <c r="T23" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="U23" s="46"/>
+      <c r="V23" s="46"/>
+      <c r="W23" s="46"/>
+      <c r="X23" s="46"/>
+      <c r="Y23" s="46"/>
+      <c r="Z23" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A24" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="B24" s="46"/>
+      <c r="C24" s="46"/>
+      <c r="D24" t="s">
+        <v>141</v>
+      </c>
+      <c r="N24" t="s">
+        <v>198</v>
+      </c>
+      <c r="T24" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A25" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="B25" s="46"/>
+      <c r="C25" s="46"/>
+      <c r="D25" t="s">
+        <v>142</v>
+      </c>
+      <c r="I25" t="s">
+        <v>169</v>
+      </c>
+      <c r="N25" t="s">
+        <v>199</v>
+      </c>
+      <c r="T25" t="s">
+        <v>228</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>143</v>
+      </c>
+      <c r="I26" t="s">
+        <v>170</v>
+      </c>
+      <c r="N26" t="s">
+        <v>200</v>
+      </c>
+      <c r="T26" t="s">
+        <v>229</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" t="s">
+        <v>144</v>
+      </c>
+      <c r="I27" t="s">
+        <v>171</v>
+      </c>
+      <c r="T27" t="s">
+        <v>230</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" t="s">
+        <v>145</v>
+      </c>
+      <c r="I28" t="s">
+        <v>172</v>
+      </c>
+      <c r="N28" t="s">
+        <v>201</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A29" s="46" t="s">
+        <v>112</v>
+      </c>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" t="s">
+        <v>146</v>
+      </c>
+      <c r="I29" t="s">
+        <v>173</v>
+      </c>
+      <c r="N29" t="s">
+        <v>202</v>
+      </c>
+      <c r="T29" t="s">
+        <v>231</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A30" s="46" t="s">
+        <v>113</v>
+      </c>
+      <c r="B30" s="46"/>
+      <c r="C30" s="46"/>
+      <c r="D30" t="s">
+        <v>147</v>
+      </c>
+      <c r="I30" t="s">
+        <v>174</v>
+      </c>
+      <c r="T30" t="s">
+        <v>232</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>114</v>
+      </c>
+      <c r="I31" s="46" t="s">
+        <v>175</v>
+      </c>
+      <c r="J31" s="46"/>
+      <c r="K31" s="46"/>
+      <c r="L31" s="46"/>
+      <c r="M31" s="46"/>
+      <c r="N31" s="46" t="s">
+        <v>203</v>
+      </c>
+      <c r="O31" s="46"/>
+      <c r="P31" s="46"/>
+      <c r="T31" t="s">
+        <v>233</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>115</v>
+      </c>
+      <c r="N32" t="s">
+        <v>204</v>
+      </c>
+      <c r="Z32" s="46" t="s">
+        <v>263</v>
+      </c>
+      <c r="AA32" s="46"/>
+      <c r="AB32" s="46"/>
+      <c r="AC32" s="46"/>
+      <c r="AD32" s="46"/>
+    </row>
+    <row r="33" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A33" s="46" t="s">
+        <v>116</v>
+      </c>
+      <c r="B33" s="46"/>
+      <c r="C33" s="46"/>
+      <c r="N33" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="34" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>117</v>
+      </c>
+      <c r="I34" t="s">
+        <v>176</v>
+      </c>
+      <c r="N34" t="s">
+        <v>206</v>
+      </c>
+      <c r="Z34" s="46" t="s">
+        <v>264</v>
+      </c>
+      <c r="AA34" s="46"/>
+      <c r="AB34" s="46"/>
+      <c r="AC34" s="46"/>
+      <c r="AD34" s="46"/>
+    </row>
+    <row r="35" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="I35" t="s">
+        <v>177</v>
+      </c>
+      <c r="N35" s="46" t="s">
+        <v>207</v>
+      </c>
+      <c r="O35" s="46"/>
+      <c r="P35" s="46"/>
+      <c r="T35" t="s">
+        <v>234</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED37D482-83EB-714D-B143-55F3284911A1}">
   <dimension ref="A1:E2"/>
   <sheetViews>

</xml_diff>